<commit_message>
Verificações, novos cards e mvp pronto
</commit_message>
<xml_diff>
--- a/downloads/Nova_ficha.xlsx
+++ b/downloads/Nova_ficha.xlsx
@@ -1148,7 +1148,7 @@
       </c>
       <c r="B4" s="61" t="inlineStr">
         <is>
-          <t>ABDIAS KELLY DE PAIVA NETO</t>
+          <t>LAURIENE VARGAS DO PRADO RODRIGUES</t>
         </is>
       </c>
       <c r="C4" s="59" t="n"/>
@@ -1188,7 +1188,7 @@
         </is>
       </c>
       <c r="B5" s="31" t="n">
-        <v>4130</v>
+        <v>4293</v>
       </c>
       <c r="C5" s="59" t="n"/>
       <c r="D5" s="64" t="n"/>
@@ -1565,22 +1565,22 @@
     <row r="27" ht="84" customHeight="1" s="54">
       <c r="A27" s="18" t="inlineStr">
         <is>
-          <t>28/02/2024</t>
+          <t>05/03/2024</t>
         </is>
       </c>
       <c r="B27" s="19" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C27" s="20" t="inlineStr">
         <is>
-          <t>500883 - CORRENTE ELO ZEBRADA 3/16 (PARA DEMARCAÇÃO) (M)</t>
+          <t>700178 - ROUPA / MACACÃO DE PROTEÇÃO (Un)</t>
         </is>
       </c>
       <c r="D27" s="21" t="n"/>
       <c r="E27" s="21" t="n"/>
       <c r="F27" s="21" t="inlineStr">
         <is>
-          <t>Dano</t>
+          <t>Primeira Entrega</t>
         </is>
       </c>
       <c r="G27" s="79" t="n"/>

</xml_diff>

<commit_message>
Campo de Operador enviando conforme a Lista
</commit_message>
<xml_diff>
--- a/downloads/Nova_ficha.xlsx
+++ b/downloads/Nova_ficha.xlsx
@@ -388,7 +388,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
@@ -581,9 +581,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -690,9 +687,9 @@
   </oneCellAnchor>
   <oneCellAnchor>
     <from>
-      <col>6</col>
+      <col>1</col>
       <colOff>0</colOff>
-      <row>27</row>
+      <row>21</row>
       <rowOff>0</rowOff>
     </from>
     <ext cx="1428750" cy="1238250"/>
@@ -703,106 +700,6 @@
       </nvPicPr>
       <blipFill>
         <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId2"/>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>6</col>
-      <colOff>0</colOff>
-      <row>28</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="1428750" cy="1238250"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="3" name="Image 3" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId3"/>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>6</col>
-      <colOff>0</colOff>
-      <row>29</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="1428750" cy="1238250"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="4" name="Image 4" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId4"/>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>6</col>
-      <colOff>0</colOff>
-      <row>30</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="1428750" cy="1238250"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="5" name="Image 5" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId5"/>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>1</col>
-      <colOff>0</colOff>
-      <row>21</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="1428750" cy="1238250"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="6" name="Image 6" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId6"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
@@ -1222,7 +1119,7 @@
       </c>
       <c r="B4" s="60" t="inlineStr">
         <is>
-          <t>THIERRY DE ALMEIDA MESQUITA</t>
+          <t>ANTONIO CARLOS SILVA DO NASCIMENTO</t>
         </is>
       </c>
       <c r="C4" s="58" t="n"/>
@@ -1262,7 +1159,7 @@
         </is>
       </c>
       <c r="B5" s="32" t="n">
-        <v>4392</v>
+        <v>4066</v>
       </c>
       <c r="C5" s="58" t="n"/>
       <c r="D5" s="63" t="n"/>
@@ -1297,7 +1194,7 @@
       </c>
       <c r="B6" s="32" t="inlineStr">
         <is>
-          <t>ASSISTENTE DE T.I</t>
+          <t>SOLDADOR 5</t>
         </is>
       </c>
       <c r="C6" s="58" t="n"/>
@@ -1315,7 +1212,7 @@
       </c>
       <c r="B7" s="33" t="inlineStr">
         <is>
-          <t>09/10/2023</t>
+          <t>14/07/2017</t>
         </is>
       </c>
       <c r="C7" s="58" t="n"/>
@@ -1333,7 +1230,7 @@
       </c>
       <c r="B8" s="65" t="inlineStr">
         <is>
-          <t>T.I - MANUNTECAO - REDE</t>
+          <t>SOLDA</t>
         </is>
       </c>
       <c r="C8" s="58" t="n"/>
@@ -1646,310 +1543,231 @@
     <row r="27" ht="84" customHeight="1" s="53">
       <c r="A27" s="17" t="inlineStr">
         <is>
-          <t>13/03/2024</t>
+          <t>15/04/2024</t>
         </is>
       </c>
       <c r="B27" s="18" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C27" s="19" t="inlineStr">
         <is>
-          <t>702020 - LUVA CANO CURTO (Un)</t>
+          <t>702008 - AVENTAL DE COURO C/ MANGAS (Un)</t>
         </is>
       </c>
       <c r="D27" s="20" t="n"/>
       <c r="E27" s="20" t="n"/>
       <c r="F27" s="20" t="inlineStr">
         <is>
-          <t>Perda</t>
+          <t>Substituição</t>
         </is>
       </c>
       <c r="G27" s="77" t="n"/>
       <c r="H27" s="59" t="n"/>
     </row>
-    <row r="28" ht="84" customHeight="1" s="53">
-      <c r="A28" s="17" t="inlineStr">
-        <is>
-          <t>18/03/2024</t>
-        </is>
-      </c>
-      <c r="B28" s="78" t="n">
-        <v>1</v>
-      </c>
-      <c r="C28" s="19" t="inlineStr">
-        <is>
-          <t>700361 - TRAVAQUEDA CORDA 12MM EXTENSOR FITA (Un)</t>
-        </is>
-      </c>
-      <c r="D28" s="20" t="n"/>
-      <c r="E28" s="20" t="n"/>
-      <c r="F28" s="20" t="inlineStr">
-        <is>
-          <t>Primeira Entrega</t>
-        </is>
-      </c>
-      <c r="G28" s="77" t="n"/>
-      <c r="H28" s="59" t="n"/>
-    </row>
-    <row r="29" ht="84" customHeight="1" s="53">
-      <c r="A29" s="17" t="inlineStr">
-        <is>
-          <t>18/03/2024</t>
-        </is>
-      </c>
-      <c r="B29" s="78" t="n">
-        <v>1</v>
-      </c>
-      <c r="C29" s="19" t="inlineStr">
-        <is>
-          <t>700361 - TRAVAQUEDA CORDA 12MM EXTENSOR FITA (Un)</t>
-        </is>
-      </c>
-      <c r="D29" s="20" t="n"/>
-      <c r="E29" s="20" t="n"/>
-      <c r="F29" s="20" t="inlineStr">
-        <is>
-          <t>Substituição</t>
-        </is>
-      </c>
-      <c r="G29" s="77" t="n"/>
-      <c r="H29" s="59" t="n"/>
-    </row>
-    <row r="30" ht="84" customHeight="1" s="53">
-      <c r="A30" s="17" t="inlineStr">
-        <is>
-          <t>18/03/2024</t>
-        </is>
-      </c>
-      <c r="B30" s="78" t="n">
-        <v>2</v>
-      </c>
-      <c r="C30" s="19" t="inlineStr">
-        <is>
-          <t>700123 - TALABARTE P/ CINTO PARAQ. NYLON TRAVA DUPLA MGS CINTOS-1879D1 (Un)</t>
-        </is>
-      </c>
-      <c r="D30" s="20" t="n"/>
-      <c r="E30" s="20" t="n"/>
-      <c r="F30" s="20" t="inlineStr">
-        <is>
-          <t>Dano</t>
-        </is>
-      </c>
-      <c r="G30" s="77" t="n"/>
-      <c r="H30" s="59" t="n"/>
-    </row>
-    <row r="31" ht="84" customHeight="1" s="53">
-      <c r="A31" s="17" t="inlineStr">
-        <is>
-          <t>18/03/2024</t>
-        </is>
-      </c>
-      <c r="B31" s="78" t="n">
-        <v>1</v>
-      </c>
-      <c r="C31" s="19" t="inlineStr">
-        <is>
-          <t>700123 - TALABARTE P/ CINTO PARAQ. NYLON TRAVA DUPLA MGS CINTOS-1879D1 (Un)</t>
-        </is>
-      </c>
-      <c r="D31" s="20" t="n"/>
-      <c r="E31" s="20" t="n"/>
-      <c r="F31" s="20" t="inlineStr">
-        <is>
-          <t>Substituição</t>
-        </is>
-      </c>
-      <c r="G31" s="77" t="n"/>
-      <c r="H31" s="59" t="n"/>
+    <row r="28" ht="18.75" customHeight="1" s="53">
+      <c r="B28" s="16" t="n"/>
+      <c r="G28" s="56" t="n"/>
+      <c r="H28" s="56" t="n"/>
+    </row>
+    <row r="29" ht="18.75" customHeight="1" s="53">
+      <c r="B29" s="16" t="n"/>
+      <c r="G29" s="78" t="n"/>
+    </row>
+    <row r="30" ht="18.75" customHeight="1" s="53">
+      <c r="B30" s="16" t="n"/>
+      <c r="G30" s="78" t="n"/>
+    </row>
+    <row r="31" ht="18.75" customHeight="1" s="53">
+      <c r="B31" s="16" t="n"/>
+      <c r="G31" s="78" t="n"/>
     </row>
     <row r="32" ht="18.75" customHeight="1" s="53">
       <c r="B32" s="16" t="n"/>
-      <c r="G32" s="79" t="n"/>
+      <c r="G32" s="78" t="n"/>
     </row>
     <row r="33" ht="18.75" customHeight="1" s="53">
       <c r="B33" s="16" t="n"/>
-      <c r="G33" s="79" t="n"/>
+      <c r="G33" s="78" t="n"/>
     </row>
     <row r="34" ht="15.75" customHeight="1" s="53">
       <c r="B34" s="16" t="n"/>
-      <c r="G34" s="79" t="n"/>
+      <c r="G34" s="78" t="n"/>
     </row>
     <row r="35" ht="15.75" customHeight="1" s="53">
       <c r="B35" s="16" t="n"/>
-      <c r="G35" s="79" t="n"/>
+      <c r="G35" s="78" t="n"/>
     </row>
     <row r="36" ht="15.75" customHeight="1" s="53">
       <c r="B36" s="16" t="n"/>
-      <c r="G36" s="79" t="n"/>
+      <c r="G36" s="78" t="n"/>
     </row>
     <row r="37" ht="15.75" customHeight="1" s="53">
       <c r="B37" s="16" t="n"/>
-      <c r="G37" s="79" t="n"/>
+      <c r="G37" s="78" t="n"/>
     </row>
     <row r="38" ht="15.75" customHeight="1" s="53">
       <c r="B38" s="16" t="n"/>
-      <c r="G38" s="79" t="n"/>
+      <c r="G38" s="78" t="n"/>
     </row>
     <row r="39" ht="15.75" customHeight="1" s="53">
       <c r="B39" s="16" t="n"/>
-      <c r="G39" s="79" t="n"/>
+      <c r="G39" s="78" t="n"/>
     </row>
     <row r="40" ht="15.75" customHeight="1" s="53">
       <c r="B40" s="16" t="n"/>
-      <c r="G40" s="79" t="n"/>
+      <c r="G40" s="78" t="n"/>
     </row>
     <row r="41" ht="15.75" customHeight="1" s="53">
       <c r="B41" s="16" t="n"/>
-      <c r="G41" s="79" t="n"/>
+      <c r="G41" s="78" t="n"/>
     </row>
     <row r="42" ht="15.75" customHeight="1" s="53">
       <c r="B42" s="16" t="n"/>
-      <c r="G42" s="79" t="n"/>
+      <c r="G42" s="78" t="n"/>
     </row>
     <row r="43" ht="15.75" customHeight="1" s="53">
       <c r="B43" s="16" t="n"/>
-      <c r="G43" s="79" t="n"/>
+      <c r="G43" s="78" t="n"/>
     </row>
     <row r="44" ht="15.75" customHeight="1" s="53">
       <c r="B44" s="16" t="n"/>
-      <c r="G44" s="79" t="n"/>
+      <c r="G44" s="78" t="n"/>
     </row>
     <row r="45" ht="15.75" customHeight="1" s="53">
       <c r="B45" s="16" t="n"/>
-      <c r="G45" s="79" t="n"/>
+      <c r="G45" s="78" t="n"/>
     </row>
     <row r="46" ht="15.75" customHeight="1" s="53">
       <c r="B46" s="16" t="n"/>
-      <c r="G46" s="79" t="n"/>
+      <c r="G46" s="78" t="n"/>
     </row>
     <row r="47" ht="15.75" customHeight="1" s="53">
       <c r="B47" s="16" t="n"/>
-      <c r="G47" s="79" t="n"/>
+      <c r="G47" s="78" t="n"/>
     </row>
     <row r="48" ht="15.75" customHeight="1" s="53">
       <c r="B48" s="16" t="n"/>
-      <c r="G48" s="79" t="n"/>
+      <c r="G48" s="78" t="n"/>
     </row>
     <row r="49" ht="15.75" customHeight="1" s="53">
       <c r="B49" s="16" t="n"/>
-      <c r="G49" s="79" t="n"/>
+      <c r="G49" s="78" t="n"/>
     </row>
     <row r="50" ht="15.75" customHeight="1" s="53">
       <c r="B50" s="16" t="n"/>
-      <c r="G50" s="79" t="n"/>
+      <c r="G50" s="78" t="n"/>
     </row>
     <row r="51" ht="15.75" customHeight="1" s="53">
       <c r="B51" s="16" t="n"/>
-      <c r="G51" s="79" t="n"/>
+      <c r="G51" s="78" t="n"/>
     </row>
     <row r="52" ht="15.75" customHeight="1" s="53">
       <c r="B52" s="16" t="n"/>
-      <c r="G52" s="79" t="n"/>
+      <c r="G52" s="78" t="n"/>
     </row>
     <row r="53" ht="15.75" customHeight="1" s="53">
       <c r="B53" s="16" t="n"/>
-      <c r="G53" s="79" t="n"/>
+      <c r="G53" s="78" t="n"/>
     </row>
     <row r="54" ht="15.75" customHeight="1" s="53">
       <c r="B54" s="16" t="n"/>
-      <c r="G54" s="79" t="n"/>
+      <c r="G54" s="78" t="n"/>
     </row>
     <row r="55" ht="15.75" customHeight="1" s="53">
       <c r="B55" s="16" t="n"/>
-      <c r="G55" s="79" t="n"/>
+      <c r="G55" s="78" t="n"/>
     </row>
     <row r="56" ht="15.75" customHeight="1" s="53">
       <c r="B56" s="16" t="n"/>
-      <c r="G56" s="79" t="n"/>
+      <c r="G56" s="78" t="n"/>
     </row>
     <row r="57" ht="15.75" customHeight="1" s="53">
       <c r="B57" s="16" t="n"/>
-      <c r="G57" s="79" t="n"/>
+      <c r="G57" s="78" t="n"/>
     </row>
     <row r="58" ht="15.75" customHeight="1" s="53">
       <c r="B58" s="16" t="n"/>
-      <c r="G58" s="79" t="n"/>
+      <c r="G58" s="78" t="n"/>
     </row>
     <row r="59" ht="15.75" customHeight="1" s="53">
       <c r="B59" s="16" t="n"/>
-      <c r="G59" s="79" t="n"/>
+      <c r="G59" s="78" t="n"/>
     </row>
     <row r="60" ht="15.75" customHeight="1" s="53">
       <c r="B60" s="16" t="n"/>
-      <c r="G60" s="79" t="n"/>
+      <c r="G60" s="78" t="n"/>
     </row>
     <row r="61" ht="15.75" customHeight="1" s="53">
       <c r="B61" s="16" t="n"/>
-      <c r="G61" s="79" t="n"/>
+      <c r="G61" s="78" t="n"/>
     </row>
     <row r="62" ht="15.75" customHeight="1" s="53">
       <c r="B62" s="16" t="n"/>
-      <c r="G62" s="79" t="n"/>
+      <c r="G62" s="78" t="n"/>
     </row>
     <row r="63" ht="15.75" customHeight="1" s="53">
       <c r="B63" s="16" t="n"/>
-      <c r="G63" s="79" t="n"/>
+      <c r="G63" s="78" t="n"/>
     </row>
     <row r="64" ht="15.75" customHeight="1" s="53">
       <c r="B64" s="16" t="n"/>
-      <c r="G64" s="79" t="n"/>
+      <c r="G64" s="78" t="n"/>
     </row>
     <row r="65" ht="15.75" customHeight="1" s="53">
       <c r="B65" s="16" t="n"/>
-      <c r="G65" s="79" t="n"/>
+      <c r="G65" s="78" t="n"/>
     </row>
     <row r="66" ht="15.75" customHeight="1" s="53">
       <c r="B66" s="16" t="n"/>
-      <c r="G66" s="79" t="n"/>
+      <c r="G66" s="78" t="n"/>
     </row>
     <row r="67" ht="15.75" customHeight="1" s="53">
       <c r="B67" s="16" t="n"/>
-      <c r="G67" s="79" t="n"/>
+      <c r="G67" s="78" t="n"/>
     </row>
     <row r="68" ht="15.75" customHeight="1" s="53">
       <c r="B68" s="16" t="n"/>
-      <c r="G68" s="79" t="n"/>
+      <c r="G68" s="78" t="n"/>
     </row>
     <row r="69" ht="15.75" customHeight="1" s="53">
       <c r="B69" s="16" t="n"/>
-      <c r="G69" s="79" t="n"/>
+      <c r="G69" s="78" t="n"/>
     </row>
     <row r="70" ht="15.75" customHeight="1" s="53">
       <c r="B70" s="16" t="n"/>
-      <c r="G70" s="79" t="n"/>
+      <c r="G70" s="78" t="n"/>
     </row>
     <row r="71" ht="15.75" customHeight="1" s="53">
       <c r="B71" s="16" t="n"/>
-      <c r="G71" s="79" t="n"/>
+      <c r="G71" s="78" t="n"/>
     </row>
     <row r="72" ht="15.75" customHeight="1" s="53">
       <c r="B72" s="16" t="n"/>
-      <c r="G72" s="79" t="n"/>
+      <c r="G72" s="78" t="n"/>
     </row>
     <row r="73" ht="15.75" customHeight="1" s="53">
       <c r="B73" s="16" t="n"/>
-      <c r="G73" s="79" t="n"/>
+      <c r="G73" s="78" t="n"/>
     </row>
     <row r="74" ht="15.75" customHeight="1" s="53">
       <c r="B74" s="16" t="n"/>
-      <c r="G74" s="79" t="n"/>
+      <c r="G74" s="78" t="n"/>
     </row>
     <row r="75" ht="15.75" customHeight="1" s="53">
       <c r="B75" s="16" t="n"/>
-      <c r="G75" s="79" t="n"/>
+      <c r="G75" s="78" t="n"/>
     </row>
     <row r="76" ht="15.75" customHeight="1" s="53">
       <c r="B76" s="16" t="n"/>
-      <c r="G76" s="79" t="n"/>
+      <c r="G76" s="78" t="n"/>
     </row>
     <row r="77" ht="15.75" customHeight="1" s="53">
       <c r="B77" s="16" t="n"/>
-      <c r="G77" s="79" t="n"/>
+      <c r="G77" s="78" t="n"/>
     </row>
     <row r="78" ht="15.75" customHeight="1" s="53">
       <c r="B78" s="16" t="n"/>
-      <c r="G78" s="79" t="n"/>
+      <c r="G78" s="78" t="n"/>
     </row>
     <row r="79" ht="15.75" customHeight="1" s="53">
       <c r="B79" s="8" t="n"/>

</xml_diff>

<commit_message>
Adicionando campo de Observação e terminando a parte de adicionar equipamento depois de criado
</commit_message>
<xml_diff>
--- a/downloads/Nova_ficha.xlsx
+++ b/downloads/Nova_ficha.xlsx
@@ -1119,7 +1119,7 @@
       </c>
       <c r="B4" s="60" t="inlineStr">
         <is>
-          <t>ANTONIO CARLOS SILVA DO NASCIMENTO</t>
+          <t>KATYLENE COELHO DA SILVA</t>
         </is>
       </c>
       <c r="C4" s="58" t="n"/>
@@ -1159,7 +1159,7 @@
         </is>
       </c>
       <c r="B5" s="32" t="n">
-        <v>4066</v>
+        <v>4114</v>
       </c>
       <c r="C5" s="58" t="n"/>
       <c r="D5" s="63" t="n"/>
@@ -1194,7 +1194,7 @@
       </c>
       <c r="B6" s="32" t="inlineStr">
         <is>
-          <t>SOLDADOR 5</t>
+          <t>SUPERVISOR (A) COMERCIAL</t>
         </is>
       </c>
       <c r="C6" s="58" t="n"/>
@@ -1212,7 +1212,7 @@
       </c>
       <c r="B7" s="33" t="inlineStr">
         <is>
-          <t>14/07/2017</t>
+          <t>24/01/2019</t>
         </is>
       </c>
       <c r="C7" s="58" t="n"/>
@@ -1230,7 +1230,7 @@
       </c>
       <c r="B8" s="65" t="inlineStr">
         <is>
-          <t>SOLDA</t>
+          <t>COMERCIAL</t>
         </is>
       </c>
       <c r="C8" s="58" t="n"/>
@@ -1543,7 +1543,7 @@
     <row r="27" ht="84" customHeight="1" s="53">
       <c r="A27" s="17" t="inlineStr">
         <is>
-          <t>15/04/2024</t>
+          <t>04/06/2024</t>
         </is>
       </c>
       <c r="B27" s="18" t="n">
@@ -1551,7 +1551,7 @@
       </c>
       <c r="C27" s="19" t="inlineStr">
         <is>
-          <t>702008 - AVENTAL DE COURO C/ MANGAS (Un)</t>
+          <t>702122 - PROTETOR AURICULAR (Un)</t>
         </is>
       </c>
       <c r="D27" s="20" t="n"/>

</xml_diff>

<commit_message>
campo para criar,deletar e alterar equipamentos
</commit_message>
<xml_diff>
--- a/downloads/Nova_ficha.xlsx
+++ b/downloads/Nova_ficha.xlsx
@@ -388,7 +388,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
@@ -581,6 +581,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -687,9 +690,9 @@
   </oneCellAnchor>
   <oneCellAnchor>
     <from>
-      <col>1</col>
+      <col>6</col>
       <colOff>0</colOff>
-      <row>21</row>
+      <row>27</row>
       <rowOff>0</rowOff>
     </from>
     <ext cx="1428750" cy="1238250"/>
@@ -700,6 +703,181 @@
       </nvPicPr>
       <blipFill>
         <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId2"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>6</col>
+      <colOff>0</colOff>
+      <row>28</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="1428750" cy="1238250"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="3" name="Image 3" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId3"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>6</col>
+      <colOff>0</colOff>
+      <row>29</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="1428750" cy="1238250"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="4" name="Image 4" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId4"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>6</col>
+      <colOff>0</colOff>
+      <row>30</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="1428750" cy="1238250"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="5" name="Image 5" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId5"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>6</col>
+      <colOff>0</colOff>
+      <row>31</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="1428750" cy="1238250"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="6" name="Image 6" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId6"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>6</col>
+      <colOff>0</colOff>
+      <row>32</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="1428750" cy="1238250"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="7" name="Image 7" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId7"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>6</col>
+      <colOff>0</colOff>
+      <row>33</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="1428750" cy="1238250"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="8" name="Image 8" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId8"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>1</col>
+      <colOff>0</colOff>
+      <row>21</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="1428750" cy="1238250"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="9" name="Image 9" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId9"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
@@ -1119,7 +1297,7 @@
       </c>
       <c r="B4" s="60" t="inlineStr">
         <is>
-          <t>KATYLENE COELHO DA SILVA</t>
+          <t>FRANCISCO LUCAS TEIXEIRA TELES</t>
         </is>
       </c>
       <c r="C4" s="58" t="n"/>
@@ -1159,7 +1337,7 @@
         </is>
       </c>
       <c r="B5" s="32" t="n">
-        <v>4114</v>
+        <v>4271</v>
       </c>
       <c r="C5" s="58" t="n"/>
       <c r="D5" s="63" t="n"/>
@@ -1194,7 +1372,7 @@
       </c>
       <c r="B6" s="32" t="inlineStr">
         <is>
-          <t>SUPERVISOR (A) COMERCIAL</t>
+          <t>SUPERVISOR OP. 3 (PINTURA)</t>
         </is>
       </c>
       <c r="C6" s="58" t="n"/>
@@ -1212,7 +1390,7 @@
       </c>
       <c r="B7" s="33" t="inlineStr">
         <is>
-          <t>24/01/2019</t>
+          <t>25/01/2021</t>
         </is>
       </c>
       <c r="C7" s="58" t="n"/>
@@ -1230,7 +1408,7 @@
       </c>
       <c r="B8" s="65" t="inlineStr">
         <is>
-          <t>COMERCIAL</t>
+          <t>PINTURA</t>
         </is>
       </c>
       <c r="C8" s="58" t="n"/>
@@ -1543,7 +1721,7 @@
     <row r="27" ht="84" customHeight="1" s="53">
       <c r="A27" s="17" t="inlineStr">
         <is>
-          <t>04/06/2024</t>
+          <t>19/04/2024</t>
         </is>
       </c>
       <c r="B27" s="18" t="n">
@@ -1564,210 +1742,349 @@
       <c r="G27" s="77" t="n"/>
       <c r="H27" s="59" t="n"/>
     </row>
-    <row r="28" ht="18.75" customHeight="1" s="53">
-      <c r="B28" s="16" t="n"/>
-      <c r="G28" s="56" t="n"/>
-      <c r="H28" s="56" t="n"/>
-    </row>
-    <row r="29" ht="18.75" customHeight="1" s="53">
-      <c r="B29" s="16" t="n"/>
-      <c r="G29" s="78" t="n"/>
-    </row>
-    <row r="30" ht="18.75" customHeight="1" s="53">
-      <c r="B30" s="16" t="n"/>
-      <c r="G30" s="78" t="n"/>
-    </row>
-    <row r="31" ht="18.75" customHeight="1" s="53">
-      <c r="B31" s="16" t="n"/>
-      <c r="G31" s="78" t="n"/>
-    </row>
-    <row r="32" ht="18.75" customHeight="1" s="53">
-      <c r="B32" s="16" t="n"/>
-      <c r="G32" s="78" t="n"/>
-    </row>
-    <row r="33" ht="18.75" customHeight="1" s="53">
-      <c r="B33" s="16" t="n"/>
-      <c r="G33" s="78" t="n"/>
-    </row>
-    <row r="34" ht="15.75" customHeight="1" s="53">
-      <c r="B34" s="16" t="n"/>
-      <c r="G34" s="78" t="n"/>
+    <row r="28" ht="84" customHeight="1" s="53">
+      <c r="A28" s="17" t="inlineStr">
+        <is>
+          <t>19/04/2024</t>
+        </is>
+      </c>
+      <c r="B28" s="78" t="n">
+        <v>1</v>
+      </c>
+      <c r="C28" s="19" t="inlineStr">
+        <is>
+          <t>702017 - LUVA DE VAQUETA C.CURTO (Un)</t>
+        </is>
+      </c>
+      <c r="D28" s="20" t="n"/>
+      <c r="E28" s="20" t="n"/>
+      <c r="F28" s="20" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
+      <c r="G28" s="77" t="n"/>
+      <c r="H28" s="59" t="n"/>
+    </row>
+    <row r="29" ht="84" customHeight="1" s="53">
+      <c r="A29" s="17" t="inlineStr">
+        <is>
+          <t>19/04/2024</t>
+        </is>
+      </c>
+      <c r="B29" s="78" t="n">
+        <v>1</v>
+      </c>
+      <c r="C29" s="19" t="inlineStr">
+        <is>
+          <t>702025 - LUVA TRICOTADA DE ALGODÃO (Un)</t>
+        </is>
+      </c>
+      <c r="D29" s="20" t="n"/>
+      <c r="E29" s="20" t="n"/>
+      <c r="F29" s="20" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
+      <c r="G29" s="77" t="n"/>
+      <c r="H29" s="59" t="n"/>
+    </row>
+    <row r="30" ht="84" customHeight="1" s="53">
+      <c r="A30" s="17" t="inlineStr">
+        <is>
+          <t>30/04/2024</t>
+        </is>
+      </c>
+      <c r="B30" s="78" t="n">
+        <v>1</v>
+      </c>
+      <c r="C30" s="19" t="inlineStr">
+        <is>
+          <t>702025 - LUVA TRICOTADA DE ALGODÃO (Un)</t>
+        </is>
+      </c>
+      <c r="D30" s="20" t="n"/>
+      <c r="E30" s="20" t="n"/>
+      <c r="F30" s="20" t="inlineStr">
+        <is>
+          <t>Substituição</t>
+        </is>
+      </c>
+      <c r="G30" s="77" t="n"/>
+      <c r="H30" s="59" t="n"/>
+    </row>
+    <row r="31" ht="84" customHeight="1" s="53">
+      <c r="A31" s="17" t="inlineStr">
+        <is>
+          <t>24/05/2024</t>
+        </is>
+      </c>
+      <c r="B31" s="78" t="n">
+        <v>1</v>
+      </c>
+      <c r="C31" s="19" t="inlineStr">
+        <is>
+          <t>702078 - OCULOS VISION 3000 INCOLOR (Un)</t>
+        </is>
+      </c>
+      <c r="D31" s="20" t="n"/>
+      <c r="E31" s="20" t="n"/>
+      <c r="F31" s="20" t="inlineStr">
+        <is>
+          <t>Substituição</t>
+        </is>
+      </c>
+      <c r="G31" s="77" t="n"/>
+      <c r="H31" s="59" t="n"/>
+    </row>
+    <row r="32" ht="84" customHeight="1" s="53">
+      <c r="A32" s="17" t="inlineStr">
+        <is>
+          <t>06/06/2024</t>
+        </is>
+      </c>
+      <c r="B32" s="78" t="n">
+        <v>1</v>
+      </c>
+      <c r="C32" s="19" t="inlineStr">
+        <is>
+          <t>702122 - PROTETOR AURICULAR (Un)</t>
+        </is>
+      </c>
+      <c r="D32" s="20" t="n"/>
+      <c r="E32" s="20" t="n"/>
+      <c r="F32" s="20" t="inlineStr">
+        <is>
+          <t>Substituição</t>
+        </is>
+      </c>
+      <c r="G32" s="77" t="n"/>
+      <c r="H32" s="59" t="n"/>
+    </row>
+    <row r="33" ht="84" customHeight="1" s="53">
+      <c r="A33" s="17" t="inlineStr">
+        <is>
+          <t>06/06/2024</t>
+        </is>
+      </c>
+      <c r="B33" s="78" t="n">
+        <v>2</v>
+      </c>
+      <c r="C33" s="19" t="inlineStr">
+        <is>
+          <t>702017 - LUVA DE VAQUETA C.CURTO (Un)</t>
+        </is>
+      </c>
+      <c r="D33" s="20" t="n"/>
+      <c r="E33" s="20" t="n"/>
+      <c r="F33" s="20" t="inlineStr">
+        <is>
+          <t>Primeira Entrega</t>
+        </is>
+      </c>
+      <c r="G33" s="77" t="n"/>
+      <c r="H33" s="59" t="n"/>
+    </row>
+    <row r="34" ht="84" customHeight="1" s="53">
+      <c r="A34" s="17" t="inlineStr">
+        <is>
+          <t>06/06/2024</t>
+        </is>
+      </c>
+      <c r="B34" s="78" t="n">
+        <v>2</v>
+      </c>
+      <c r="C34" s="19" t="inlineStr">
+        <is>
+          <t>702057 - RESP. DESC. PFF2 (Un)</t>
+        </is>
+      </c>
+      <c r="D34" s="20" t="n"/>
+      <c r="E34" s="20" t="n"/>
+      <c r="F34" s="20" t="inlineStr">
+        <is>
+          <t>Primeira Entrega</t>
+        </is>
+      </c>
+      <c r="G34" s="77" t="n"/>
+      <c r="H34" s="59" t="n"/>
     </row>
     <row r="35" ht="15.75" customHeight="1" s="53">
       <c r="B35" s="16" t="n"/>
-      <c r="G35" s="78" t="n"/>
+      <c r="G35" s="79" t="n"/>
     </row>
     <row r="36" ht="15.75" customHeight="1" s="53">
       <c r="B36" s="16" t="n"/>
-      <c r="G36" s="78" t="n"/>
+      <c r="G36" s="79" t="n"/>
     </row>
     <row r="37" ht="15.75" customHeight="1" s="53">
       <c r="B37" s="16" t="n"/>
-      <c r="G37" s="78" t="n"/>
+      <c r="G37" s="79" t="n"/>
     </row>
     <row r="38" ht="15.75" customHeight="1" s="53">
       <c r="B38" s="16" t="n"/>
-      <c r="G38" s="78" t="n"/>
+      <c r="G38" s="79" t="n"/>
     </row>
     <row r="39" ht="15.75" customHeight="1" s="53">
       <c r="B39" s="16" t="n"/>
-      <c r="G39" s="78" t="n"/>
+      <c r="G39" s="79" t="n"/>
     </row>
     <row r="40" ht="15.75" customHeight="1" s="53">
       <c r="B40" s="16" t="n"/>
-      <c r="G40" s="78" t="n"/>
+      <c r="G40" s="79" t="n"/>
     </row>
     <row r="41" ht="15.75" customHeight="1" s="53">
       <c r="B41" s="16" t="n"/>
-      <c r="G41" s="78" t="n"/>
+      <c r="G41" s="79" t="n"/>
     </row>
     <row r="42" ht="15.75" customHeight="1" s="53">
       <c r="B42" s="16" t="n"/>
-      <c r="G42" s="78" t="n"/>
+      <c r="G42" s="79" t="n"/>
     </row>
     <row r="43" ht="15.75" customHeight="1" s="53">
       <c r="B43" s="16" t="n"/>
-      <c r="G43" s="78" t="n"/>
+      <c r="G43" s="79" t="n"/>
     </row>
     <row r="44" ht="15.75" customHeight="1" s="53">
       <c r="B44" s="16" t="n"/>
-      <c r="G44" s="78" t="n"/>
+      <c r="G44" s="79" t="n"/>
     </row>
     <row r="45" ht="15.75" customHeight="1" s="53">
       <c r="B45" s="16" t="n"/>
-      <c r="G45" s="78" t="n"/>
+      <c r="G45" s="79" t="n"/>
     </row>
     <row r="46" ht="15.75" customHeight="1" s="53">
       <c r="B46" s="16" t="n"/>
-      <c r="G46" s="78" t="n"/>
+      <c r="G46" s="79" t="n"/>
     </row>
     <row r="47" ht="15.75" customHeight="1" s="53">
       <c r="B47" s="16" t="n"/>
-      <c r="G47" s="78" t="n"/>
+      <c r="G47" s="79" t="n"/>
     </row>
     <row r="48" ht="15.75" customHeight="1" s="53">
       <c r="B48" s="16" t="n"/>
-      <c r="G48" s="78" t="n"/>
+      <c r="G48" s="79" t="n"/>
     </row>
     <row r="49" ht="15.75" customHeight="1" s="53">
       <c r="B49" s="16" t="n"/>
-      <c r="G49" s="78" t="n"/>
+      <c r="G49" s="79" t="n"/>
     </row>
     <row r="50" ht="15.75" customHeight="1" s="53">
       <c r="B50" s="16" t="n"/>
-      <c r="G50" s="78" t="n"/>
+      <c r="G50" s="79" t="n"/>
     </row>
     <row r="51" ht="15.75" customHeight="1" s="53">
       <c r="B51" s="16" t="n"/>
-      <c r="G51" s="78" t="n"/>
+      <c r="G51" s="79" t="n"/>
     </row>
     <row r="52" ht="15.75" customHeight="1" s="53">
       <c r="B52" s="16" t="n"/>
-      <c r="G52" s="78" t="n"/>
+      <c r="G52" s="79" t="n"/>
     </row>
     <row r="53" ht="15.75" customHeight="1" s="53">
       <c r="B53" s="16" t="n"/>
-      <c r="G53" s="78" t="n"/>
+      <c r="G53" s="79" t="n"/>
     </row>
     <row r="54" ht="15.75" customHeight="1" s="53">
       <c r="B54" s="16" t="n"/>
-      <c r="G54" s="78" t="n"/>
+      <c r="G54" s="79" t="n"/>
     </row>
     <row r="55" ht="15.75" customHeight="1" s="53">
       <c r="B55" s="16" t="n"/>
-      <c r="G55" s="78" t="n"/>
+      <c r="G55" s="79" t="n"/>
     </row>
     <row r="56" ht="15.75" customHeight="1" s="53">
       <c r="B56" s="16" t="n"/>
-      <c r="G56" s="78" t="n"/>
+      <c r="G56" s="79" t="n"/>
     </row>
     <row r="57" ht="15.75" customHeight="1" s="53">
       <c r="B57" s="16" t="n"/>
-      <c r="G57" s="78" t="n"/>
+      <c r="G57" s="79" t="n"/>
     </row>
     <row r="58" ht="15.75" customHeight="1" s="53">
       <c r="B58" s="16" t="n"/>
-      <c r="G58" s="78" t="n"/>
+      <c r="G58" s="79" t="n"/>
     </row>
     <row r="59" ht="15.75" customHeight="1" s="53">
       <c r="B59" s="16" t="n"/>
-      <c r="G59" s="78" t="n"/>
+      <c r="G59" s="79" t="n"/>
     </row>
     <row r="60" ht="15.75" customHeight="1" s="53">
       <c r="B60" s="16" t="n"/>
-      <c r="G60" s="78" t="n"/>
+      <c r="G60" s="79" t="n"/>
     </row>
     <row r="61" ht="15.75" customHeight="1" s="53">
       <c r="B61" s="16" t="n"/>
-      <c r="G61" s="78" t="n"/>
+      <c r="G61" s="79" t="n"/>
     </row>
     <row r="62" ht="15.75" customHeight="1" s="53">
       <c r="B62" s="16" t="n"/>
-      <c r="G62" s="78" t="n"/>
+      <c r="G62" s="79" t="n"/>
     </row>
     <row r="63" ht="15.75" customHeight="1" s="53">
       <c r="B63" s="16" t="n"/>
-      <c r="G63" s="78" t="n"/>
+      <c r="G63" s="79" t="n"/>
     </row>
     <row r="64" ht="15.75" customHeight="1" s="53">
       <c r="B64" s="16" t="n"/>
-      <c r="G64" s="78" t="n"/>
+      <c r="G64" s="79" t="n"/>
     </row>
     <row r="65" ht="15.75" customHeight="1" s="53">
       <c r="B65" s="16" t="n"/>
-      <c r="G65" s="78" t="n"/>
+      <c r="G65" s="79" t="n"/>
     </row>
     <row r="66" ht="15.75" customHeight="1" s="53">
       <c r="B66" s="16" t="n"/>
-      <c r="G66" s="78" t="n"/>
+      <c r="G66" s="79" t="n"/>
     </row>
     <row r="67" ht="15.75" customHeight="1" s="53">
       <c r="B67" s="16" t="n"/>
-      <c r="G67" s="78" t="n"/>
+      <c r="G67" s="79" t="n"/>
     </row>
     <row r="68" ht="15.75" customHeight="1" s="53">
       <c r="B68" s="16" t="n"/>
-      <c r="G68" s="78" t="n"/>
+      <c r="G68" s="79" t="n"/>
     </row>
     <row r="69" ht="15.75" customHeight="1" s="53">
       <c r="B69" s="16" t="n"/>
-      <c r="G69" s="78" t="n"/>
+      <c r="G69" s="79" t="n"/>
     </row>
     <row r="70" ht="15.75" customHeight="1" s="53">
       <c r="B70" s="16" t="n"/>
-      <c r="G70" s="78" t="n"/>
+      <c r="G70" s="79" t="n"/>
     </row>
     <row r="71" ht="15.75" customHeight="1" s="53">
       <c r="B71" s="16" t="n"/>
-      <c r="G71" s="78" t="n"/>
+      <c r="G71" s="79" t="n"/>
     </row>
     <row r="72" ht="15.75" customHeight="1" s="53">
       <c r="B72" s="16" t="n"/>
-      <c r="G72" s="78" t="n"/>
+      <c r="G72" s="79" t="n"/>
     </row>
     <row r="73" ht="15.75" customHeight="1" s="53">
       <c r="B73" s="16" t="n"/>
-      <c r="G73" s="78" t="n"/>
+      <c r="G73" s="79" t="n"/>
     </row>
     <row r="74" ht="15.75" customHeight="1" s="53">
       <c r="B74" s="16" t="n"/>
-      <c r="G74" s="78" t="n"/>
+      <c r="G74" s="79" t="n"/>
     </row>
     <row r="75" ht="15.75" customHeight="1" s="53">
       <c r="B75" s="16" t="n"/>
-      <c r="G75" s="78" t="n"/>
+      <c r="G75" s="79" t="n"/>
     </row>
     <row r="76" ht="15.75" customHeight="1" s="53">
       <c r="B76" s="16" t="n"/>
-      <c r="G76" s="78" t="n"/>
+      <c r="G76" s="79" t="n"/>
     </row>
     <row r="77" ht="15.75" customHeight="1" s="53">
       <c r="B77" s="16" t="n"/>
-      <c r="G77" s="78" t="n"/>
+      <c r="G77" s="79" t="n"/>
     </row>
     <row r="78" ht="15.75" customHeight="1" s="53">
       <c r="B78" s="16" t="n"/>
-      <c r="G78" s="78" t="n"/>
+      <c r="G78" s="79" t="n"/>
     </row>
     <row r="79" ht="15.75" customHeight="1" s="53">
       <c r="B79" s="8" t="n"/>

</xml_diff>

<commit_message>
Alterando dados na Ficha e finalizando o CRUD de equipamentos
</commit_message>
<xml_diff>
--- a/downloads/Nova_ficha.xlsx
+++ b/downloads/Nova_ficha.xlsx
@@ -865,9 +865,9 @@
   </oneCellAnchor>
   <oneCellAnchor>
     <from>
-      <col>1</col>
+      <col>6</col>
       <colOff>0</colOff>
-      <row>21</row>
+      <row>34</row>
       <rowOff>0</rowOff>
     </from>
     <ext cx="1428750" cy="1238250"/>
@@ -878,6 +878,356 @@
       </nvPicPr>
       <blipFill>
         <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId9"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>6</col>
+      <colOff>0</colOff>
+      <row>35</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="1428750" cy="1238250"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="10" name="Image 10" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId10"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>6</col>
+      <colOff>0</colOff>
+      <row>36</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="1428750" cy="1238250"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="11" name="Image 11" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId11"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>6</col>
+      <colOff>0</colOff>
+      <row>37</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="1428750" cy="1238250"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="12" name="Image 12" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId12"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>6</col>
+      <colOff>0</colOff>
+      <row>38</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="1428750" cy="1238250"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="13" name="Image 13" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId13"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>6</col>
+      <colOff>0</colOff>
+      <row>39</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="1428750" cy="1238250"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="14" name="Image 14" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId14"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>6</col>
+      <colOff>0</colOff>
+      <row>40</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="1428750" cy="1238250"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="15" name="Image 15" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId15"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>6</col>
+      <colOff>0</colOff>
+      <row>41</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="1428750" cy="1238250"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="16" name="Image 16" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId16"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>6</col>
+      <colOff>0</colOff>
+      <row>42</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="1428750" cy="1238250"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="17" name="Image 17" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId17"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>6</col>
+      <colOff>0</colOff>
+      <row>43</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="1428750" cy="1238250"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="18" name="Image 18" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId18"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>6</col>
+      <colOff>0</colOff>
+      <row>44</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="1428750" cy="1238250"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="19" name="Image 19" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId19"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>6</col>
+      <colOff>0</colOff>
+      <row>45</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="1428750" cy="1238250"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="20" name="Image 20" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId20"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>6</col>
+      <colOff>0</colOff>
+      <row>46</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="1428750" cy="1238250"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="21" name="Image 21" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId21"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>6</col>
+      <colOff>0</colOff>
+      <row>47</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="1428750" cy="1238250"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="22" name="Image 22" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId22"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>1</col>
+      <colOff>0</colOff>
+      <row>21</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="1428750" cy="1238250"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="23" name="Image 23" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId23"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
@@ -1297,7 +1647,7 @@
       </c>
       <c r="B4" s="60" t="inlineStr">
         <is>
-          <t>FRANCISCO LUCAS TEIXEIRA TELES</t>
+          <t>RAPHAEL SOUSA DA SILVA</t>
         </is>
       </c>
       <c r="C4" s="58" t="n"/>
@@ -1337,7 +1687,7 @@
         </is>
       </c>
       <c r="B5" s="32" t="n">
-        <v>4271</v>
+        <v>4420</v>
       </c>
       <c r="C5" s="58" t="n"/>
       <c r="D5" s="63" t="n"/>
@@ -1370,11 +1720,7 @@
           <t>FUNÇÃO:</t>
         </is>
       </c>
-      <c r="B6" s="32" t="inlineStr">
-        <is>
-          <t>SUPERVISOR OP. 3 (PINTURA)</t>
-        </is>
-      </c>
+      <c r="B6" s="32" t="n"/>
       <c r="C6" s="58" t="n"/>
       <c r="D6" s="63" t="n"/>
       <c r="E6" s="64" t="n"/>
@@ -1390,7 +1736,7 @@
       </c>
       <c r="B7" s="33" t="inlineStr">
         <is>
-          <t>25/01/2021</t>
+          <t>22/04/2024</t>
         </is>
       </c>
       <c r="C7" s="58" t="n"/>
@@ -1721,7 +2067,7 @@
     <row r="27" ht="84" customHeight="1" s="53">
       <c r="A27" s="17" t="inlineStr">
         <is>
-          <t>19/04/2024</t>
+          <t>02/05/2024</t>
         </is>
       </c>
       <c r="B27" s="18" t="n">
@@ -1745,7 +2091,7 @@
     <row r="28" ht="84" customHeight="1" s="53">
       <c r="A28" s="17" t="inlineStr">
         <is>
-          <t>19/04/2024</t>
+          <t>08/05/2024</t>
         </is>
       </c>
       <c r="B28" s="78" t="n">
@@ -1753,14 +2099,14 @@
       </c>
       <c r="C28" s="19" t="inlineStr">
         <is>
-          <t>702017 - LUVA DE VAQUETA C.CURTO (Un)</t>
+          <t>702067 - PROTETOR FACIAL 8 INCOLOR (Un)</t>
         </is>
       </c>
       <c r="D28" s="20" t="n"/>
       <c r="E28" s="20" t="n"/>
       <c r="F28" s="20" t="inlineStr">
         <is>
-          <t>Perda</t>
+          <t>Substituição</t>
         </is>
       </c>
       <c r="G28" s="77" t="n"/>
@@ -1769,7 +2115,7 @@
     <row r="29" ht="84" customHeight="1" s="53">
       <c r="A29" s="17" t="inlineStr">
         <is>
-          <t>19/04/2024</t>
+          <t>08/05/2024</t>
         </is>
       </c>
       <c r="B29" s="78" t="n">
@@ -1777,23 +2123,19 @@
       </c>
       <c r="C29" s="19" t="inlineStr">
         <is>
-          <t>702025 - LUVA TRICOTADA DE ALGODÃO (Un)</t>
+          <t>702110 - MANGOTE P/SOLDADOR (Un)</t>
         </is>
       </c>
       <c r="D29" s="20" t="n"/>
       <c r="E29" s="20" t="n"/>
-      <c r="F29" s="20" t="inlineStr">
-        <is>
-          <t>Perda</t>
-        </is>
-      </c>
+      <c r="F29" s="20" t="n"/>
       <c r="G29" s="77" t="n"/>
       <c r="H29" s="59" t="n"/>
     </row>
     <row r="30" ht="84" customHeight="1" s="53">
       <c r="A30" s="17" t="inlineStr">
         <is>
-          <t>30/04/2024</t>
+          <t>08/05/2024</t>
         </is>
       </c>
       <c r="B30" s="78" t="n">
@@ -1801,47 +2143,39 @@
       </c>
       <c r="C30" s="19" t="inlineStr">
         <is>
-          <t>702025 - LUVA TRICOTADA DE ALGODÃO (Un)</t>
+          <t>702006 - AVENTAL DE COURO SIMPLES (Un)</t>
         </is>
       </c>
       <c r="D30" s="20" t="n"/>
       <c r="E30" s="20" t="n"/>
-      <c r="F30" s="20" t="inlineStr">
-        <is>
-          <t>Substituição</t>
-        </is>
-      </c>
+      <c r="F30" s="20" t="n"/>
       <c r="G30" s="77" t="n"/>
       <c r="H30" s="59" t="n"/>
     </row>
     <row r="31" ht="84" customHeight="1" s="53">
       <c r="A31" s="17" t="inlineStr">
         <is>
-          <t>24/05/2024</t>
+          <t>10/05/2024</t>
         </is>
       </c>
       <c r="B31" s="78" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C31" s="19" t="inlineStr">
         <is>
-          <t>702078 - OCULOS VISION 3000 INCOLOR (Un)</t>
+          <t>702020 - LUVA CANO CURTO (Un)</t>
         </is>
       </c>
       <c r="D31" s="20" t="n"/>
       <c r="E31" s="20" t="n"/>
-      <c r="F31" s="20" t="inlineStr">
-        <is>
-          <t>Substituição</t>
-        </is>
-      </c>
+      <c r="F31" s="20" t="n"/>
       <c r="G31" s="77" t="n"/>
       <c r="H31" s="59" t="n"/>
     </row>
     <row r="32" ht="84" customHeight="1" s="53">
       <c r="A32" s="17" t="inlineStr">
         <is>
-          <t>06/06/2024</t>
+          <t>10/05/2024</t>
         </is>
       </c>
       <c r="B32" s="78" t="n">
@@ -1849,23 +2183,19 @@
       </c>
       <c r="C32" s="19" t="inlineStr">
         <is>
-          <t>702122 - PROTETOR AURICULAR (Un)</t>
+          <t>702057 - RESP. DESC. PFF2 (Un)</t>
         </is>
       </c>
       <c r="D32" s="20" t="n"/>
       <c r="E32" s="20" t="n"/>
-      <c r="F32" s="20" t="inlineStr">
-        <is>
-          <t>Substituição</t>
-        </is>
-      </c>
+      <c r="F32" s="20" t="n"/>
       <c r="G32" s="77" t="n"/>
       <c r="H32" s="59" t="n"/>
     </row>
     <row r="33" ht="84" customHeight="1" s="53">
       <c r="A33" s="17" t="inlineStr">
         <is>
-          <t>06/06/2024</t>
+          <t>24/05/2024</t>
         </is>
       </c>
       <c r="B33" s="78" t="n">
@@ -1880,7 +2210,7 @@
       <c r="E33" s="20" t="n"/>
       <c r="F33" s="20" t="inlineStr">
         <is>
-          <t>Primeira Entrega</t>
+          <t>Substituição</t>
         </is>
       </c>
       <c r="G33" s="77" t="n"/>
@@ -1889,7 +2219,7 @@
     <row r="34" ht="84" customHeight="1" s="53">
       <c r="A34" s="17" t="inlineStr">
         <is>
-          <t>06/06/2024</t>
+          <t>24/05/2024</t>
         </is>
       </c>
       <c r="B34" s="78" t="n">
@@ -1897,74 +2227,322 @@
       </c>
       <c r="C34" s="19" t="inlineStr">
         <is>
-          <t>702057 - RESP. DESC. PFF2 (Un)</t>
+          <t>702032 - LUVA PVC C/LONGO FORRADA (Un)</t>
         </is>
       </c>
       <c r="D34" s="20" t="n"/>
       <c r="E34" s="20" t="n"/>
       <c r="F34" s="20" t="inlineStr">
         <is>
-          <t>Primeira Entrega</t>
+          <t>Substituição</t>
         </is>
       </c>
       <c r="G34" s="77" t="n"/>
       <c r="H34" s="59" t="n"/>
     </row>
-    <row r="35" ht="15.75" customHeight="1" s="53">
-      <c r="B35" s="16" t="n"/>
-      <c r="G35" s="79" t="n"/>
-    </row>
-    <row r="36" ht="15.75" customHeight="1" s="53">
-      <c r="B36" s="16" t="n"/>
-      <c r="G36" s="79" t="n"/>
-    </row>
-    <row r="37" ht="15.75" customHeight="1" s="53">
-      <c r="B37" s="16" t="n"/>
-      <c r="G37" s="79" t="n"/>
-    </row>
-    <row r="38" ht="15.75" customHeight="1" s="53">
-      <c r="B38" s="16" t="n"/>
-      <c r="G38" s="79" t="n"/>
-    </row>
-    <row r="39" ht="15.75" customHeight="1" s="53">
-      <c r="B39" s="16" t="n"/>
-      <c r="G39" s="79" t="n"/>
-    </row>
-    <row r="40" ht="15.75" customHeight="1" s="53">
-      <c r="B40" s="16" t="n"/>
-      <c r="G40" s="79" t="n"/>
-    </row>
-    <row r="41" ht="15.75" customHeight="1" s="53">
-      <c r="B41" s="16" t="n"/>
-      <c r="G41" s="79" t="n"/>
-    </row>
-    <row r="42" ht="15.75" customHeight="1" s="53">
-      <c r="B42" s="16" t="n"/>
-      <c r="G42" s="79" t="n"/>
-    </row>
-    <row r="43" ht="15.75" customHeight="1" s="53">
-      <c r="B43" s="16" t="n"/>
-      <c r="G43" s="79" t="n"/>
-    </row>
-    <row r="44" ht="15.75" customHeight="1" s="53">
-      <c r="B44" s="16" t="n"/>
-      <c r="G44" s="79" t="n"/>
-    </row>
-    <row r="45" ht="15.75" customHeight="1" s="53">
-      <c r="B45" s="16" t="n"/>
-      <c r="G45" s="79" t="n"/>
-    </row>
-    <row r="46" ht="15.75" customHeight="1" s="53">
-      <c r="B46" s="16" t="n"/>
-      <c r="G46" s="79" t="n"/>
-    </row>
-    <row r="47" ht="15.75" customHeight="1" s="53">
-      <c r="B47" s="16" t="n"/>
-      <c r="G47" s="79" t="n"/>
-    </row>
-    <row r="48" ht="15.75" customHeight="1" s="53">
-      <c r="B48" s="16" t="n"/>
-      <c r="G48" s="79" t="n"/>
+    <row r="35" ht="84" customHeight="1" s="53">
+      <c r="A35" s="17" t="inlineStr">
+        <is>
+          <t>24/05/2024</t>
+        </is>
+      </c>
+      <c r="B35" s="78" t="n">
+        <v>1</v>
+      </c>
+      <c r="C35" s="19" t="inlineStr">
+        <is>
+          <t>702134 - OCULOS SOBREPOR INCOLOR (Un)</t>
+        </is>
+      </c>
+      <c r="D35" s="20" t="n"/>
+      <c r="E35" s="20" t="n"/>
+      <c r="F35" s="20" t="n"/>
+      <c r="G35" s="77" t="n"/>
+      <c r="H35" s="59" t="n"/>
+    </row>
+    <row r="36" ht="84" customHeight="1" s="53">
+      <c r="A36" s="17" t="inlineStr">
+        <is>
+          <t>13/06/2024</t>
+        </is>
+      </c>
+      <c r="B36" s="78" t="n">
+        <v>2</v>
+      </c>
+      <c r="C36" s="19" t="inlineStr">
+        <is>
+          <t>702017 - LUVA DE VAQUETA C.CURTO (Un)</t>
+        </is>
+      </c>
+      <c r="D36" s="20" t="n"/>
+      <c r="E36" s="20" t="n"/>
+      <c r="F36" s="20" t="inlineStr">
+        <is>
+          <t>Substituição</t>
+        </is>
+      </c>
+      <c r="G36" s="77" t="n"/>
+      <c r="H36" s="59" t="n"/>
+    </row>
+    <row r="37" ht="84" customHeight="1" s="53">
+      <c r="A37" s="17" t="inlineStr">
+        <is>
+          <t>14/06/2024</t>
+        </is>
+      </c>
+      <c r="B37" s="78" t="n">
+        <v>2</v>
+      </c>
+      <c r="C37" s="19" t="inlineStr">
+        <is>
+          <t>702032 - LUVA PVC C/LONGO FORRADA (Un)</t>
+        </is>
+      </c>
+      <c r="D37" s="20" t="n"/>
+      <c r="E37" s="20" t="n"/>
+      <c r="F37" s="20" t="inlineStr">
+        <is>
+          <t>Substituição</t>
+        </is>
+      </c>
+      <c r="G37" s="77" t="n"/>
+      <c r="H37" s="59" t="n"/>
+    </row>
+    <row r="38" ht="84" customHeight="1" s="53">
+      <c r="A38" s="17" t="inlineStr">
+        <is>
+          <t>14/06/2024</t>
+        </is>
+      </c>
+      <c r="B38" s="78" t="n">
+        <v>2</v>
+      </c>
+      <c r="C38" s="19" t="inlineStr">
+        <is>
+          <t>702025 - LUVA TRICOTADA DE ALGODÃO (Un)</t>
+        </is>
+      </c>
+      <c r="D38" s="20" t="n"/>
+      <c r="E38" s="20" t="n"/>
+      <c r="F38" s="20" t="inlineStr">
+        <is>
+          <t>Substituição</t>
+        </is>
+      </c>
+      <c r="G38" s="77" t="n"/>
+      <c r="H38" s="59" t="n"/>
+    </row>
+    <row r="39" ht="84" customHeight="1" s="53">
+      <c r="A39" s="17" t="inlineStr">
+        <is>
+          <t>17/06/2024</t>
+        </is>
+      </c>
+      <c r="B39" s="78" t="n">
+        <v>1</v>
+      </c>
+      <c r="C39" s="19" t="inlineStr">
+        <is>
+          <t>702067 - PROTETOR FACIAL 8 INCOLOR (Un)</t>
+        </is>
+      </c>
+      <c r="D39" s="20" t="n"/>
+      <c r="E39" s="20" t="n"/>
+      <c r="F39" s="20" t="n"/>
+      <c r="G39" s="77" t="n"/>
+      <c r="H39" s="59" t="n"/>
+    </row>
+    <row r="40" ht="84" customHeight="1" s="53">
+      <c r="A40" s="17" t="inlineStr">
+        <is>
+          <t>17/06/2024</t>
+        </is>
+      </c>
+      <c r="B40" s="78" t="n">
+        <v>2</v>
+      </c>
+      <c r="C40" s="19" t="inlineStr">
+        <is>
+          <t>702111 - MANGOTE DE TECIDO C/ ELASTICO NOS PUNHOS (Un)</t>
+        </is>
+      </c>
+      <c r="D40" s="20" t="n"/>
+      <c r="E40" s="20" t="n"/>
+      <c r="F40" s="20" t="n"/>
+      <c r="G40" s="77" t="n"/>
+      <c r="H40" s="59" t="n"/>
+    </row>
+    <row r="41" ht="84" customHeight="1" s="53">
+      <c r="A41" s="17" t="inlineStr">
+        <is>
+          <t>17/06/2024</t>
+        </is>
+      </c>
+      <c r="B41" s="78" t="n">
+        <v>1</v>
+      </c>
+      <c r="C41" s="19" t="inlineStr">
+        <is>
+          <t>702122 - PROTETOR AURICULAR (Un)</t>
+        </is>
+      </c>
+      <c r="D41" s="20" t="n"/>
+      <c r="E41" s="20" t="n"/>
+      <c r="F41" s="20" t="n"/>
+      <c r="G41" s="77" t="n"/>
+      <c r="H41" s="59" t="n"/>
+    </row>
+    <row r="42" ht="84" customHeight="1" s="53">
+      <c r="A42" s="17" t="inlineStr">
+        <is>
+          <t>21/06/2024</t>
+        </is>
+      </c>
+      <c r="B42" s="78" t="n">
+        <v>2</v>
+      </c>
+      <c r="C42" s="19" t="inlineStr">
+        <is>
+          <t>702017 - LUVA DE VAQUETA C.CURTO (Un)</t>
+        </is>
+      </c>
+      <c r="D42" s="20" t="n"/>
+      <c r="E42" s="20" t="n"/>
+      <c r="F42" s="20" t="inlineStr">
+        <is>
+          <t>Substituição</t>
+        </is>
+      </c>
+      <c r="G42" s="77" t="n"/>
+      <c r="H42" s="59" t="n"/>
+    </row>
+    <row r="43" ht="84" customHeight="1" s="53">
+      <c r="A43" s="17" t="inlineStr">
+        <is>
+          <t>21/06/2024</t>
+        </is>
+      </c>
+      <c r="B43" s="78" t="n">
+        <v>2</v>
+      </c>
+      <c r="C43" s="19" t="inlineStr">
+        <is>
+          <t>702032 - LUVA PVC C/LONGO FORRADA (Un)</t>
+        </is>
+      </c>
+      <c r="D43" s="20" t="n"/>
+      <c r="E43" s="20" t="n"/>
+      <c r="F43" s="20" t="inlineStr">
+        <is>
+          <t>Substituição</t>
+        </is>
+      </c>
+      <c r="G43" s="77" t="n"/>
+      <c r="H43" s="59" t="n"/>
+    </row>
+    <row r="44" ht="84" customHeight="1" s="53">
+      <c r="A44" s="17" t="inlineStr">
+        <is>
+          <t>21/06/2024</t>
+        </is>
+      </c>
+      <c r="B44" s="78" t="n">
+        <v>2</v>
+      </c>
+      <c r="C44" s="19" t="inlineStr">
+        <is>
+          <t>702025 - LUVA TRICOTADA DE ALGODÃO (Un)</t>
+        </is>
+      </c>
+      <c r="D44" s="20" t="n"/>
+      <c r="E44" s="20" t="n"/>
+      <c r="F44" s="20" t="inlineStr">
+        <is>
+          <t>Substituição</t>
+        </is>
+      </c>
+      <c r="G44" s="77" t="n"/>
+      <c r="H44" s="59" t="n"/>
+    </row>
+    <row r="45" ht="84" customHeight="1" s="53">
+      <c r="A45" s="17" t="inlineStr">
+        <is>
+          <t>28/06/2024</t>
+        </is>
+      </c>
+      <c r="B45" s="78" t="n">
+        <v>2</v>
+      </c>
+      <c r="C45" s="19" t="inlineStr">
+        <is>
+          <t>702111 - MANGOTE DE TECIDO C/ ELASTICO NOS PUNHOS (Un)</t>
+        </is>
+      </c>
+      <c r="D45" s="20" t="n"/>
+      <c r="E45" s="20" t="n"/>
+      <c r="F45" s="20" t="n"/>
+      <c r="G45" s="77" t="n"/>
+      <c r="H45" s="59" t="n"/>
+    </row>
+    <row r="46" ht="84" customHeight="1" s="53">
+      <c r="A46" s="17" t="inlineStr">
+        <is>
+          <t>28/06/2024</t>
+        </is>
+      </c>
+      <c r="B46" s="78" t="n">
+        <v>2</v>
+      </c>
+      <c r="C46" s="19" t="inlineStr">
+        <is>
+          <t>702032 - LUVA PVC C/LONGO FORRADA (Un)</t>
+        </is>
+      </c>
+      <c r="D46" s="20" t="n"/>
+      <c r="E46" s="20" t="n"/>
+      <c r="F46" s="20" t="n"/>
+      <c r="G46" s="77" t="n"/>
+      <c r="H46" s="59" t="n"/>
+    </row>
+    <row r="47" ht="84" customHeight="1" s="53">
+      <c r="A47" s="17" t="inlineStr">
+        <is>
+          <t>28/06/2024</t>
+        </is>
+      </c>
+      <c r="B47" s="78" t="n">
+        <v>2</v>
+      </c>
+      <c r="C47" s="19" t="inlineStr">
+        <is>
+          <t>702025 - LUVA TRICOTADA DE ALGODÃO (Un)</t>
+        </is>
+      </c>
+      <c r="D47" s="20" t="n"/>
+      <c r="E47" s="20" t="n"/>
+      <c r="F47" s="20" t="n"/>
+      <c r="G47" s="77" t="n"/>
+      <c r="H47" s="59" t="n"/>
+    </row>
+    <row r="48" ht="84" customHeight="1" s="53">
+      <c r="A48" s="17" t="inlineStr">
+        <is>
+          <t>28/06/2024</t>
+        </is>
+      </c>
+      <c r="B48" s="78" t="n">
+        <v>2</v>
+      </c>
+      <c r="C48" s="19" t="inlineStr">
+        <is>
+          <t>702017 - LUVA DE VAQUETA C.CURTO (Un)</t>
+        </is>
+      </c>
+      <c r="D48" s="20" t="n"/>
+      <c r="E48" s="20" t="n"/>
+      <c r="F48" s="20" t="n"/>
+      <c r="G48" s="77" t="n"/>
+      <c r="H48" s="59" t="n"/>
     </row>
     <row r="49" ht="15.75" customHeight="1" s="53">
       <c r="B49" s="16" t="n"/>

</xml_diff>

<commit_message>
habilitando campos de quantidade e obs na edicao de padroes
</commit_message>
<xml_diff>
--- a/downloads/Nova_ficha.xlsx
+++ b/downloads/Nova_ficha.xlsx
@@ -715,9 +715,9 @@
   </oneCellAnchor>
   <oneCellAnchor>
     <from>
-      <col>6</col>
+      <col>1</col>
       <colOff>0</colOff>
-      <row>28</row>
+      <row>21</row>
       <rowOff>0</rowOff>
     </from>
     <ext cx="1428750" cy="1238250"/>
@@ -728,506 +728,6 @@
       </nvPicPr>
       <blipFill>
         <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId3"/>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>6</col>
-      <colOff>0</colOff>
-      <row>29</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="1428750" cy="1238250"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="4" name="Image 4" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId4"/>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>6</col>
-      <colOff>0</colOff>
-      <row>30</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="1428750" cy="1238250"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="5" name="Image 5" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId5"/>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>6</col>
-      <colOff>0</colOff>
-      <row>31</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="1428750" cy="1238250"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="6" name="Image 6" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId6"/>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>6</col>
-      <colOff>0</colOff>
-      <row>32</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="1428750" cy="1238250"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="7" name="Image 7" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId7"/>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>6</col>
-      <colOff>0</colOff>
-      <row>33</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="1428750" cy="1238250"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="8" name="Image 8" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId8"/>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>6</col>
-      <colOff>0</colOff>
-      <row>34</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="1428750" cy="1238250"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="9" name="Image 9" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId9"/>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>6</col>
-      <colOff>0</colOff>
-      <row>35</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="1428750" cy="1238250"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="10" name="Image 10" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId10"/>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>6</col>
-      <colOff>0</colOff>
-      <row>36</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="1428750" cy="1238250"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="11" name="Image 11" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId11"/>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>6</col>
-      <colOff>0</colOff>
-      <row>37</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="1428750" cy="1238250"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="12" name="Image 12" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId12"/>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>6</col>
-      <colOff>0</colOff>
-      <row>38</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="1428750" cy="1238250"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="13" name="Image 13" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId13"/>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>6</col>
-      <colOff>0</colOff>
-      <row>39</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="1428750" cy="1238250"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="14" name="Image 14" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId14"/>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>6</col>
-      <colOff>0</colOff>
-      <row>40</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="1428750" cy="1238250"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="15" name="Image 15" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId15"/>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>6</col>
-      <colOff>0</colOff>
-      <row>41</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="1428750" cy="1238250"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="16" name="Image 16" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId16"/>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>6</col>
-      <colOff>0</colOff>
-      <row>42</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="1428750" cy="1238250"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="17" name="Image 17" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId17"/>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>6</col>
-      <colOff>0</colOff>
-      <row>43</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="1428750" cy="1238250"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="18" name="Image 18" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId18"/>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>6</col>
-      <colOff>0</colOff>
-      <row>44</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="1428750" cy="1238250"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="19" name="Image 19" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId19"/>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>6</col>
-      <colOff>0</colOff>
-      <row>45</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="1428750" cy="1238250"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="20" name="Image 20" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId20"/>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>6</col>
-      <colOff>0</colOff>
-      <row>46</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="1428750" cy="1238250"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="21" name="Image 21" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId21"/>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>6</col>
-      <colOff>0</colOff>
-      <row>47</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="1428750" cy="1238250"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="22" name="Image 22" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId22"/>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>1</col>
-      <colOff>0</colOff>
-      <row>21</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="1428750" cy="1238250"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="23" name="Image 23" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId23"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
@@ -1647,7 +1147,7 @@
       </c>
       <c r="B4" s="60" t="inlineStr">
         <is>
-          <t>RAPHAEL SOUSA DA SILVA</t>
+          <t>SAUL SANTOS MARINHO</t>
         </is>
       </c>
       <c r="C4" s="58" t="n"/>
@@ -1687,7 +1187,7 @@
         </is>
       </c>
       <c r="B5" s="32" t="n">
-        <v>4420</v>
+        <v>4405</v>
       </c>
       <c r="C5" s="58" t="n"/>
       <c r="D5" s="63" t="n"/>
@@ -1720,7 +1220,11 @@
           <t>FUNÇÃO:</t>
         </is>
       </c>
-      <c r="B6" s="32" t="n"/>
+      <c r="B6" s="32" t="inlineStr">
+        <is>
+          <t>ASSISTENTE DE DESENVOLVIMENTO DE SISTEMAS</t>
+        </is>
+      </c>
       <c r="C6" s="58" t="n"/>
       <c r="D6" s="63" t="n"/>
       <c r="E6" s="64" t="n"/>
@@ -1736,7 +1240,7 @@
       </c>
       <c r="B7" s="33" t="inlineStr">
         <is>
-          <t>22/04/2024</t>
+          <t>01/03/2024</t>
         </is>
       </c>
       <c r="C7" s="58" t="n"/>
@@ -1754,7 +1258,7 @@
       </c>
       <c r="B8" s="65" t="inlineStr">
         <is>
-          <t>PINTURA</t>
+          <t>T.I - DESENVOLVIMENTO</t>
         </is>
       </c>
       <c r="C8" s="58" t="n"/>
@@ -2067,31 +1571,29 @@
     <row r="27" ht="84" customHeight="1" s="53">
       <c r="A27" s="17" t="inlineStr">
         <is>
-          <t>02/05/2024</t>
+          <t>02/09/2024</t>
         </is>
       </c>
       <c r="B27" s="18" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C27" s="19" t="inlineStr">
         <is>
-          <t>702122 - PROTETOR AURICULAR (Un)</t>
+          <t>701039 - BOTAS VAQUETA C/ BIQUEIRA AÇO/COMPOSITE (Un)</t>
         </is>
       </c>
-      <c r="D27" s="20" t="n"/>
+      <c r="D27" s="20" t="n">
+        <v>36935</v>
+      </c>
       <c r="E27" s="20" t="n"/>
-      <c r="F27" s="20" t="inlineStr">
-        <is>
-          <t>Substituição</t>
-        </is>
-      </c>
+      <c r="F27" s="20" t="n"/>
       <c r="G27" s="77" t="n"/>
       <c r="H27" s="59" t="n"/>
     </row>
     <row r="28" ht="84" customHeight="1" s="53">
       <c r="A28" s="17" t="inlineStr">
         <is>
-          <t>08/05/2024</t>
+          <t>23/04/2025</t>
         </is>
       </c>
       <c r="B28" s="78" t="n">
@@ -2099,450 +1601,94 @@
       </c>
       <c r="C28" s="19" t="inlineStr">
         <is>
-          <t>702067 - PROTETOR FACIAL 8 INCOLOR (Un)</t>
+          <t>700193 - CAMISA SOCIAL MANGA CURTA (Un)</t>
         </is>
       </c>
       <c r="D28" s="20" t="n"/>
       <c r="E28" s="20" t="n"/>
-      <c r="F28" s="20" t="inlineStr">
-        <is>
-          <t>Substituição</t>
-        </is>
-      </c>
+      <c r="F28" s="20" t="n"/>
       <c r="G28" s="77" t="n"/>
       <c r="H28" s="59" t="n"/>
     </row>
-    <row r="29" ht="84" customHeight="1" s="53">
-      <c r="A29" s="17" t="inlineStr">
-        <is>
-          <t>08/05/2024</t>
-        </is>
-      </c>
-      <c r="B29" s="78" t="n">
-        <v>1</v>
-      </c>
-      <c r="C29" s="19" t="inlineStr">
-        <is>
-          <t>702110 - MANGOTE P/SOLDADOR (Un)</t>
-        </is>
-      </c>
-      <c r="D29" s="20" t="n"/>
-      <c r="E29" s="20" t="n"/>
-      <c r="F29" s="20" t="n"/>
-      <c r="G29" s="77" t="n"/>
-      <c r="H29" s="59" t="n"/>
-    </row>
-    <row r="30" ht="84" customHeight="1" s="53">
-      <c r="A30" s="17" t="inlineStr">
-        <is>
-          <t>08/05/2024</t>
-        </is>
-      </c>
-      <c r="B30" s="78" t="n">
-        <v>1</v>
-      </c>
-      <c r="C30" s="19" t="inlineStr">
-        <is>
-          <t>702006 - AVENTAL DE COURO SIMPLES (Un)</t>
-        </is>
-      </c>
-      <c r="D30" s="20" t="n"/>
-      <c r="E30" s="20" t="n"/>
-      <c r="F30" s="20" t="n"/>
-      <c r="G30" s="77" t="n"/>
-      <c r="H30" s="59" t="n"/>
-    </row>
-    <row r="31" ht="84" customHeight="1" s="53">
-      <c r="A31" s="17" t="inlineStr">
-        <is>
-          <t>10/05/2024</t>
-        </is>
-      </c>
-      <c r="B31" s="78" t="n">
-        <v>2</v>
-      </c>
-      <c r="C31" s="19" t="inlineStr">
-        <is>
-          <t>702020 - LUVA CANO CURTO (Un)</t>
-        </is>
-      </c>
-      <c r="D31" s="20" t="n"/>
-      <c r="E31" s="20" t="n"/>
-      <c r="F31" s="20" t="n"/>
-      <c r="G31" s="77" t="n"/>
-      <c r="H31" s="59" t="n"/>
-    </row>
-    <row r="32" ht="84" customHeight="1" s="53">
-      <c r="A32" s="17" t="inlineStr">
-        <is>
-          <t>10/05/2024</t>
-        </is>
-      </c>
-      <c r="B32" s="78" t="n">
-        <v>1</v>
-      </c>
-      <c r="C32" s="19" t="inlineStr">
-        <is>
-          <t>702057 - RESP. DESC. PFF2 (Un)</t>
-        </is>
-      </c>
-      <c r="D32" s="20" t="n"/>
-      <c r="E32" s="20" t="n"/>
-      <c r="F32" s="20" t="n"/>
-      <c r="G32" s="77" t="n"/>
-      <c r="H32" s="59" t="n"/>
-    </row>
-    <row r="33" ht="84" customHeight="1" s="53">
-      <c r="A33" s="17" t="inlineStr">
-        <is>
-          <t>24/05/2024</t>
-        </is>
-      </c>
-      <c r="B33" s="78" t="n">
-        <v>2</v>
-      </c>
-      <c r="C33" s="19" t="inlineStr">
-        <is>
-          <t>702017 - LUVA DE VAQUETA C.CURTO (Un)</t>
-        </is>
-      </c>
-      <c r="D33" s="20" t="n"/>
-      <c r="E33" s="20" t="n"/>
-      <c r="F33" s="20" t="inlineStr">
-        <is>
-          <t>Substituição</t>
-        </is>
-      </c>
-      <c r="G33" s="77" t="n"/>
-      <c r="H33" s="59" t="n"/>
-    </row>
-    <row r="34" ht="84" customHeight="1" s="53">
-      <c r="A34" s="17" t="inlineStr">
-        <is>
-          <t>24/05/2024</t>
-        </is>
-      </c>
-      <c r="B34" s="78" t="n">
-        <v>2</v>
-      </c>
-      <c r="C34" s="19" t="inlineStr">
-        <is>
-          <t>702032 - LUVA PVC C/LONGO FORRADA (Un)</t>
-        </is>
-      </c>
-      <c r="D34" s="20" t="n"/>
-      <c r="E34" s="20" t="n"/>
-      <c r="F34" s="20" t="inlineStr">
-        <is>
-          <t>Substituição</t>
-        </is>
-      </c>
-      <c r="G34" s="77" t="n"/>
-      <c r="H34" s="59" t="n"/>
-    </row>
-    <row r="35" ht="84" customHeight="1" s="53">
-      <c r="A35" s="17" t="inlineStr">
-        <is>
-          <t>24/05/2024</t>
-        </is>
-      </c>
-      <c r="B35" s="78" t="n">
-        <v>1</v>
-      </c>
-      <c r="C35" s="19" t="inlineStr">
-        <is>
-          <t>702134 - OCULOS SOBREPOR INCOLOR (Un)</t>
-        </is>
-      </c>
-      <c r="D35" s="20" t="n"/>
-      <c r="E35" s="20" t="n"/>
-      <c r="F35" s="20" t="n"/>
-      <c r="G35" s="77" t="n"/>
-      <c r="H35" s="59" t="n"/>
-    </row>
-    <row r="36" ht="84" customHeight="1" s="53">
-      <c r="A36" s="17" t="inlineStr">
-        <is>
-          <t>13/06/2024</t>
-        </is>
-      </c>
-      <c r="B36" s="78" t="n">
-        <v>2</v>
-      </c>
-      <c r="C36" s="19" t="inlineStr">
-        <is>
-          <t>702017 - LUVA DE VAQUETA C.CURTO (Un)</t>
-        </is>
-      </c>
-      <c r="D36" s="20" t="n"/>
-      <c r="E36" s="20" t="n"/>
-      <c r="F36" s="20" t="inlineStr">
-        <is>
-          <t>Substituição</t>
-        </is>
-      </c>
-      <c r="G36" s="77" t="n"/>
-      <c r="H36" s="59" t="n"/>
-    </row>
-    <row r="37" ht="84" customHeight="1" s="53">
-      <c r="A37" s="17" t="inlineStr">
-        <is>
-          <t>14/06/2024</t>
-        </is>
-      </c>
-      <c r="B37" s="78" t="n">
-        <v>2</v>
-      </c>
-      <c r="C37" s="19" t="inlineStr">
-        <is>
-          <t>702032 - LUVA PVC C/LONGO FORRADA (Un)</t>
-        </is>
-      </c>
-      <c r="D37" s="20" t="n"/>
-      <c r="E37" s="20" t="n"/>
-      <c r="F37" s="20" t="inlineStr">
-        <is>
-          <t>Substituição</t>
-        </is>
-      </c>
-      <c r="G37" s="77" t="n"/>
-      <c r="H37" s="59" t="n"/>
-    </row>
-    <row r="38" ht="84" customHeight="1" s="53">
-      <c r="A38" s="17" t="inlineStr">
-        <is>
-          <t>14/06/2024</t>
-        </is>
-      </c>
-      <c r="B38" s="78" t="n">
-        <v>2</v>
-      </c>
-      <c r="C38" s="19" t="inlineStr">
-        <is>
-          <t>702025 - LUVA TRICOTADA DE ALGODÃO (Un)</t>
-        </is>
-      </c>
-      <c r="D38" s="20" t="n"/>
-      <c r="E38" s="20" t="n"/>
-      <c r="F38" s="20" t="inlineStr">
-        <is>
-          <t>Substituição</t>
-        </is>
-      </c>
-      <c r="G38" s="77" t="n"/>
-      <c r="H38" s="59" t="n"/>
-    </row>
-    <row r="39" ht="84" customHeight="1" s="53">
-      <c r="A39" s="17" t="inlineStr">
-        <is>
-          <t>17/06/2024</t>
-        </is>
-      </c>
-      <c r="B39" s="78" t="n">
-        <v>1</v>
-      </c>
-      <c r="C39" s="19" t="inlineStr">
-        <is>
-          <t>702067 - PROTETOR FACIAL 8 INCOLOR (Un)</t>
-        </is>
-      </c>
-      <c r="D39" s="20" t="n"/>
-      <c r="E39" s="20" t="n"/>
-      <c r="F39" s="20" t="n"/>
-      <c r="G39" s="77" t="n"/>
-      <c r="H39" s="59" t="n"/>
-    </row>
-    <row r="40" ht="84" customHeight="1" s="53">
-      <c r="A40" s="17" t="inlineStr">
-        <is>
-          <t>17/06/2024</t>
-        </is>
-      </c>
-      <c r="B40" s="78" t="n">
-        <v>2</v>
-      </c>
-      <c r="C40" s="19" t="inlineStr">
-        <is>
-          <t>702111 - MANGOTE DE TECIDO C/ ELASTICO NOS PUNHOS (Un)</t>
-        </is>
-      </c>
-      <c r="D40" s="20" t="n"/>
-      <c r="E40" s="20" t="n"/>
-      <c r="F40" s="20" t="n"/>
-      <c r="G40" s="77" t="n"/>
-      <c r="H40" s="59" t="n"/>
-    </row>
-    <row r="41" ht="84" customHeight="1" s="53">
-      <c r="A41" s="17" t="inlineStr">
-        <is>
-          <t>17/06/2024</t>
-        </is>
-      </c>
-      <c r="B41" s="78" t="n">
-        <v>1</v>
-      </c>
-      <c r="C41" s="19" t="inlineStr">
-        <is>
-          <t>702122 - PROTETOR AURICULAR (Un)</t>
-        </is>
-      </c>
-      <c r="D41" s="20" t="n"/>
-      <c r="E41" s="20" t="n"/>
-      <c r="F41" s="20" t="n"/>
-      <c r="G41" s="77" t="n"/>
-      <c r="H41" s="59" t="n"/>
-    </row>
-    <row r="42" ht="84" customHeight="1" s="53">
-      <c r="A42" s="17" t="inlineStr">
-        <is>
-          <t>21/06/2024</t>
-        </is>
-      </c>
-      <c r="B42" s="78" t="n">
-        <v>2</v>
-      </c>
-      <c r="C42" s="19" t="inlineStr">
-        <is>
-          <t>702017 - LUVA DE VAQUETA C.CURTO (Un)</t>
-        </is>
-      </c>
-      <c r="D42" s="20" t="n"/>
-      <c r="E42" s="20" t="n"/>
-      <c r="F42" s="20" t="inlineStr">
-        <is>
-          <t>Substituição</t>
-        </is>
-      </c>
-      <c r="G42" s="77" t="n"/>
-      <c r="H42" s="59" t="n"/>
-    </row>
-    <row r="43" ht="84" customHeight="1" s="53">
-      <c r="A43" s="17" t="inlineStr">
-        <is>
-          <t>21/06/2024</t>
-        </is>
-      </c>
-      <c r="B43" s="78" t="n">
-        <v>2</v>
-      </c>
-      <c r="C43" s="19" t="inlineStr">
-        <is>
-          <t>702032 - LUVA PVC C/LONGO FORRADA (Un)</t>
-        </is>
-      </c>
-      <c r="D43" s="20" t="n"/>
-      <c r="E43" s="20" t="n"/>
-      <c r="F43" s="20" t="inlineStr">
-        <is>
-          <t>Substituição</t>
-        </is>
-      </c>
-      <c r="G43" s="77" t="n"/>
-      <c r="H43" s="59" t="n"/>
-    </row>
-    <row r="44" ht="84" customHeight="1" s="53">
-      <c r="A44" s="17" t="inlineStr">
-        <is>
-          <t>21/06/2024</t>
-        </is>
-      </c>
-      <c r="B44" s="78" t="n">
-        <v>2</v>
-      </c>
-      <c r="C44" s="19" t="inlineStr">
-        <is>
-          <t>702025 - LUVA TRICOTADA DE ALGODÃO (Un)</t>
-        </is>
-      </c>
-      <c r="D44" s="20" t="n"/>
-      <c r="E44" s="20" t="n"/>
-      <c r="F44" s="20" t="inlineStr">
-        <is>
-          <t>Substituição</t>
-        </is>
-      </c>
-      <c r="G44" s="77" t="n"/>
-      <c r="H44" s="59" t="n"/>
-    </row>
-    <row r="45" ht="84" customHeight="1" s="53">
-      <c r="A45" s="17" t="inlineStr">
-        <is>
-          <t>28/06/2024</t>
-        </is>
-      </c>
-      <c r="B45" s="78" t="n">
-        <v>2</v>
-      </c>
-      <c r="C45" s="19" t="inlineStr">
-        <is>
-          <t>702111 - MANGOTE DE TECIDO C/ ELASTICO NOS PUNHOS (Un)</t>
-        </is>
-      </c>
-      <c r="D45" s="20" t="n"/>
-      <c r="E45" s="20" t="n"/>
-      <c r="F45" s="20" t="n"/>
-      <c r="G45" s="77" t="n"/>
-      <c r="H45" s="59" t="n"/>
-    </row>
-    <row r="46" ht="84" customHeight="1" s="53">
-      <c r="A46" s="17" t="inlineStr">
-        <is>
-          <t>28/06/2024</t>
-        </is>
-      </c>
-      <c r="B46" s="78" t="n">
-        <v>2</v>
-      </c>
-      <c r="C46" s="19" t="inlineStr">
-        <is>
-          <t>702032 - LUVA PVC C/LONGO FORRADA (Un)</t>
-        </is>
-      </c>
-      <c r="D46" s="20" t="n"/>
-      <c r="E46" s="20" t="n"/>
-      <c r="F46" s="20" t="n"/>
-      <c r="G46" s="77" t="n"/>
-      <c r="H46" s="59" t="n"/>
-    </row>
-    <row r="47" ht="84" customHeight="1" s="53">
-      <c r="A47" s="17" t="inlineStr">
-        <is>
-          <t>28/06/2024</t>
-        </is>
-      </c>
-      <c r="B47" s="78" t="n">
-        <v>2</v>
-      </c>
-      <c r="C47" s="19" t="inlineStr">
-        <is>
-          <t>702025 - LUVA TRICOTADA DE ALGODÃO (Un)</t>
-        </is>
-      </c>
-      <c r="D47" s="20" t="n"/>
-      <c r="E47" s="20" t="n"/>
-      <c r="F47" s="20" t="n"/>
-      <c r="G47" s="77" t="n"/>
-      <c r="H47" s="59" t="n"/>
-    </row>
-    <row r="48" ht="84" customHeight="1" s="53">
-      <c r="A48" s="17" t="inlineStr">
-        <is>
-          <t>28/06/2024</t>
-        </is>
-      </c>
-      <c r="B48" s="78" t="n">
-        <v>2</v>
-      </c>
-      <c r="C48" s="19" t="inlineStr">
-        <is>
-          <t>702017 - LUVA DE VAQUETA C.CURTO (Un)</t>
-        </is>
-      </c>
-      <c r="D48" s="20" t="n"/>
-      <c r="E48" s="20" t="n"/>
-      <c r="F48" s="20" t="n"/>
-      <c r="G48" s="77" t="n"/>
-      <c r="H48" s="59" t="n"/>
+    <row r="29" ht="18.75" customHeight="1" s="53">
+      <c r="B29" s="16" t="n"/>
+      <c r="G29" s="79" t="n"/>
+    </row>
+    <row r="30" ht="18.75" customHeight="1" s="53">
+      <c r="B30" s="16" t="n"/>
+      <c r="G30" s="79" t="n"/>
+    </row>
+    <row r="31" ht="18.75" customHeight="1" s="53">
+      <c r="B31" s="16" t="n"/>
+      <c r="G31" s="79" t="n"/>
+    </row>
+    <row r="32" ht="18.75" customHeight="1" s="53">
+      <c r="B32" s="16" t="n"/>
+      <c r="G32" s="79" t="n"/>
+    </row>
+    <row r="33" ht="18.75" customHeight="1" s="53">
+      <c r="B33" s="16" t="n"/>
+      <c r="G33" s="79" t="n"/>
+    </row>
+    <row r="34" ht="15.75" customHeight="1" s="53">
+      <c r="B34" s="16" t="n"/>
+      <c r="G34" s="79" t="n"/>
+    </row>
+    <row r="35" ht="15.75" customHeight="1" s="53">
+      <c r="B35" s="16" t="n"/>
+      <c r="G35" s="79" t="n"/>
+    </row>
+    <row r="36" ht="15.75" customHeight="1" s="53">
+      <c r="B36" s="16" t="n"/>
+      <c r="G36" s="79" t="n"/>
+    </row>
+    <row r="37" ht="15.75" customHeight="1" s="53">
+      <c r="B37" s="16" t="n"/>
+      <c r="G37" s="79" t="n"/>
+    </row>
+    <row r="38" ht="15.75" customHeight="1" s="53">
+      <c r="B38" s="16" t="n"/>
+      <c r="G38" s="79" t="n"/>
+    </row>
+    <row r="39" ht="15.75" customHeight="1" s="53">
+      <c r="B39" s="16" t="n"/>
+      <c r="G39" s="79" t="n"/>
+    </row>
+    <row r="40" ht="15.75" customHeight="1" s="53">
+      <c r="B40" s="16" t="n"/>
+      <c r="G40" s="79" t="n"/>
+    </row>
+    <row r="41" ht="15.75" customHeight="1" s="53">
+      <c r="B41" s="16" t="n"/>
+      <c r="G41" s="79" t="n"/>
+    </row>
+    <row r="42" ht="15.75" customHeight="1" s="53">
+      <c r="B42" s="16" t="n"/>
+      <c r="G42" s="79" t="n"/>
+    </row>
+    <row r="43" ht="15.75" customHeight="1" s="53">
+      <c r="B43" s="16" t="n"/>
+      <c r="G43" s="79" t="n"/>
+    </row>
+    <row r="44" ht="15.75" customHeight="1" s="53">
+      <c r="B44" s="16" t="n"/>
+      <c r="G44" s="79" t="n"/>
+    </row>
+    <row r="45" ht="15.75" customHeight="1" s="53">
+      <c r="B45" s="16" t="n"/>
+      <c r="G45" s="79" t="n"/>
+    </row>
+    <row r="46" ht="15.75" customHeight="1" s="53">
+      <c r="B46" s="16" t="n"/>
+      <c r="G46" s="79" t="n"/>
+    </row>
+    <row r="47" ht="15.75" customHeight="1" s="53">
+      <c r="B47" s="16" t="n"/>
+      <c r="G47" s="79" t="n"/>
+    </row>
+    <row r="48" ht="15.75" customHeight="1" s="53">
+      <c r="B48" s="16" t="n"/>
+      <c r="G48" s="79" t="n"/>
     </row>
     <row r="49" ht="15.75" customHeight="1" s="53">
       <c r="B49" s="16" t="n"/>

</xml_diff>

<commit_message>
:bug: fix: Envio de Assinatura para o usuario correto
</commit_message>
<xml_diff>
--- a/downloads/Nova_ficha.xlsx
+++ b/downloads/Nova_ficha.xlsx
@@ -388,7 +388,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
@@ -581,9 +581,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -690,9 +687,9 @@
   </oneCellAnchor>
   <oneCellAnchor>
     <from>
-      <col>6</col>
+      <col>1</col>
       <colOff>0</colOff>
-      <row>27</row>
+      <row>21</row>
       <rowOff>0</rowOff>
     </from>
     <ext cx="1428750" cy="1238250"/>
@@ -703,31 +700,6 @@
       </nvPicPr>
       <blipFill>
         <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId2"/>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>1</col>
-      <colOff>0</colOff>
-      <row>21</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="1428750" cy="1238250"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="3" name="Image 3" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId3"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
@@ -1147,7 +1119,7 @@
       </c>
       <c r="B4" s="60" t="inlineStr">
         <is>
-          <t>SAUL SANTOS MARINHO</t>
+          <t>User Test 2</t>
         </is>
       </c>
       <c r="C4" s="58" t="n"/>
@@ -1187,7 +1159,7 @@
         </is>
       </c>
       <c r="B5" s="32" t="n">
-        <v>4405</v>
+        <v>9998</v>
       </c>
       <c r="C5" s="58" t="n"/>
       <c r="D5" s="63" t="n"/>
@@ -1220,11 +1192,7 @@
           <t>FUNÇÃO:</t>
         </is>
       </c>
-      <c r="B6" s="32" t="inlineStr">
-        <is>
-          <t>ASSISTENTE DE DESENVOLVIMENTO DE SISTEMAS</t>
-        </is>
-      </c>
+      <c r="B6" s="32" t="n"/>
       <c r="C6" s="58" t="n"/>
       <c r="D6" s="63" t="n"/>
       <c r="E6" s="64" t="n"/>
@@ -1240,7 +1208,7 @@
       </c>
       <c r="B7" s="33" t="inlineStr">
         <is>
-          <t>01/03/2024</t>
+          <t>12/05/2025</t>
         </is>
       </c>
       <c r="C7" s="58" t="n"/>
@@ -1571,244 +1539,227 @@
     <row r="27" ht="84" customHeight="1" s="53">
       <c r="A27" s="17" t="inlineStr">
         <is>
-          <t>02/09/2024</t>
+          <t>13/05/2025</t>
         </is>
       </c>
       <c r="B27" s="18" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C27" s="19" t="inlineStr">
         <is>
-          <t>701039 - BOTAS VAQUETA C/ BIQUEIRA AÇO/COMPOSITE (Un)</t>
+          <t>702052 - VALVULA DE INALAÇÃO 3M</t>
         </is>
       </c>
-      <c r="D27" s="20" t="n">
-        <v>36935</v>
-      </c>
+      <c r="D27" s="20" t="n"/>
       <c r="E27" s="20" t="n"/>
       <c r="F27" s="20" t="n"/>
       <c r="G27" s="77" t="n"/>
       <c r="H27" s="59" t="n"/>
     </row>
-    <row r="28" ht="84" customHeight="1" s="53">
-      <c r="A28" s="17" t="inlineStr">
-        <is>
-          <t>23/04/2025</t>
-        </is>
-      </c>
-      <c r="B28" s="78" t="n">
-        <v>1</v>
-      </c>
-      <c r="C28" s="19" t="inlineStr">
-        <is>
-          <t>700193 - CAMISA SOCIAL MANGA CURTA (Un)</t>
-        </is>
-      </c>
-      <c r="D28" s="20" t="n"/>
-      <c r="E28" s="20" t="n"/>
-      <c r="F28" s="20" t="n"/>
-      <c r="G28" s="77" t="n"/>
-      <c r="H28" s="59" t="n"/>
+    <row r="28" ht="18.75" customHeight="1" s="53">
+      <c r="B28" s="16" t="n"/>
+      <c r="G28" s="56" t="n"/>
+      <c r="H28" s="56" t="n"/>
     </row>
     <row r="29" ht="18.75" customHeight="1" s="53">
       <c r="B29" s="16" t="n"/>
-      <c r="G29" s="79" t="n"/>
+      <c r="G29" s="78" t="n"/>
     </row>
     <row r="30" ht="18.75" customHeight="1" s="53">
       <c r="B30" s="16" t="n"/>
-      <c r="G30" s="79" t="n"/>
+      <c r="G30" s="78" t="n"/>
     </row>
     <row r="31" ht="18.75" customHeight="1" s="53">
       <c r="B31" s="16" t="n"/>
-      <c r="G31" s="79" t="n"/>
+      <c r="G31" s="78" t="n"/>
     </row>
     <row r="32" ht="18.75" customHeight="1" s="53">
       <c r="B32" s="16" t="n"/>
-      <c r="G32" s="79" t="n"/>
+      <c r="G32" s="78" t="n"/>
     </row>
     <row r="33" ht="18.75" customHeight="1" s="53">
       <c r="B33" s="16" t="n"/>
-      <c r="G33" s="79" t="n"/>
+      <c r="G33" s="78" t="n"/>
     </row>
     <row r="34" ht="15.75" customHeight="1" s="53">
       <c r="B34" s="16" t="n"/>
-      <c r="G34" s="79" t="n"/>
+      <c r="G34" s="78" t="n"/>
     </row>
     <row r="35" ht="15.75" customHeight="1" s="53">
       <c r="B35" s="16" t="n"/>
-      <c r="G35" s="79" t="n"/>
+      <c r="G35" s="78" t="n"/>
     </row>
     <row r="36" ht="15.75" customHeight="1" s="53">
       <c r="B36" s="16" t="n"/>
-      <c r="G36" s="79" t="n"/>
+      <c r="G36" s="78" t="n"/>
     </row>
     <row r="37" ht="15.75" customHeight="1" s="53">
       <c r="B37" s="16" t="n"/>
-      <c r="G37" s="79" t="n"/>
+      <c r="G37" s="78" t="n"/>
     </row>
     <row r="38" ht="15.75" customHeight="1" s="53">
       <c r="B38" s="16" t="n"/>
-      <c r="G38" s="79" t="n"/>
+      <c r="G38" s="78" t="n"/>
     </row>
     <row r="39" ht="15.75" customHeight="1" s="53">
       <c r="B39" s="16" t="n"/>
-      <c r="G39" s="79" t="n"/>
+      <c r="G39" s="78" t="n"/>
     </row>
     <row r="40" ht="15.75" customHeight="1" s="53">
       <c r="B40" s="16" t="n"/>
-      <c r="G40" s="79" t="n"/>
+      <c r="G40" s="78" t="n"/>
     </row>
     <row r="41" ht="15.75" customHeight="1" s="53">
       <c r="B41" s="16" t="n"/>
-      <c r="G41" s="79" t="n"/>
+      <c r="G41" s="78" t="n"/>
     </row>
     <row r="42" ht="15.75" customHeight="1" s="53">
       <c r="B42" s="16" t="n"/>
-      <c r="G42" s="79" t="n"/>
+      <c r="G42" s="78" t="n"/>
     </row>
     <row r="43" ht="15.75" customHeight="1" s="53">
       <c r="B43" s="16" t="n"/>
-      <c r="G43" s="79" t="n"/>
+      <c r="G43" s="78" t="n"/>
     </row>
     <row r="44" ht="15.75" customHeight="1" s="53">
       <c r="B44" s="16" t="n"/>
-      <c r="G44" s="79" t="n"/>
+      <c r="G44" s="78" t="n"/>
     </row>
     <row r="45" ht="15.75" customHeight="1" s="53">
       <c r="B45" s="16" t="n"/>
-      <c r="G45" s="79" t="n"/>
+      <c r="G45" s="78" t="n"/>
     </row>
     <row r="46" ht="15.75" customHeight="1" s="53">
       <c r="B46" s="16" t="n"/>
-      <c r="G46" s="79" t="n"/>
+      <c r="G46" s="78" t="n"/>
     </row>
     <row r="47" ht="15.75" customHeight="1" s="53">
       <c r="B47" s="16" t="n"/>
-      <c r="G47" s="79" t="n"/>
+      <c r="G47" s="78" t="n"/>
     </row>
     <row r="48" ht="15.75" customHeight="1" s="53">
       <c r="B48" s="16" t="n"/>
-      <c r="G48" s="79" t="n"/>
+      <c r="G48" s="78" t="n"/>
     </row>
     <row r="49" ht="15.75" customHeight="1" s="53">
       <c r="B49" s="16" t="n"/>
-      <c r="G49" s="79" t="n"/>
+      <c r="G49" s="78" t="n"/>
     </row>
     <row r="50" ht="15.75" customHeight="1" s="53">
       <c r="B50" s="16" t="n"/>
-      <c r="G50" s="79" t="n"/>
+      <c r="G50" s="78" t="n"/>
     </row>
     <row r="51" ht="15.75" customHeight="1" s="53">
       <c r="B51" s="16" t="n"/>
-      <c r="G51" s="79" t="n"/>
+      <c r="G51" s="78" t="n"/>
     </row>
     <row r="52" ht="15.75" customHeight="1" s="53">
       <c r="B52" s="16" t="n"/>
-      <c r="G52" s="79" t="n"/>
+      <c r="G52" s="78" t="n"/>
     </row>
     <row r="53" ht="15.75" customHeight="1" s="53">
       <c r="B53" s="16" t="n"/>
-      <c r="G53" s="79" t="n"/>
+      <c r="G53" s="78" t="n"/>
     </row>
     <row r="54" ht="15.75" customHeight="1" s="53">
       <c r="B54" s="16" t="n"/>
-      <c r="G54" s="79" t="n"/>
+      <c r="G54" s="78" t="n"/>
     </row>
     <row r="55" ht="15.75" customHeight="1" s="53">
       <c r="B55" s="16" t="n"/>
-      <c r="G55" s="79" t="n"/>
+      <c r="G55" s="78" t="n"/>
     </row>
     <row r="56" ht="15.75" customHeight="1" s="53">
       <c r="B56" s="16" t="n"/>
-      <c r="G56" s="79" t="n"/>
+      <c r="G56" s="78" t="n"/>
     </row>
     <row r="57" ht="15.75" customHeight="1" s="53">
       <c r="B57" s="16" t="n"/>
-      <c r="G57" s="79" t="n"/>
+      <c r="G57" s="78" t="n"/>
     </row>
     <row r="58" ht="15.75" customHeight="1" s="53">
       <c r="B58" s="16" t="n"/>
-      <c r="G58" s="79" t="n"/>
+      <c r="G58" s="78" t="n"/>
     </row>
     <row r="59" ht="15.75" customHeight="1" s="53">
       <c r="B59" s="16" t="n"/>
-      <c r="G59" s="79" t="n"/>
+      <c r="G59" s="78" t="n"/>
     </row>
     <row r="60" ht="15.75" customHeight="1" s="53">
       <c r="B60" s="16" t="n"/>
-      <c r="G60" s="79" t="n"/>
+      <c r="G60" s="78" t="n"/>
     </row>
     <row r="61" ht="15.75" customHeight="1" s="53">
       <c r="B61" s="16" t="n"/>
-      <c r="G61" s="79" t="n"/>
+      <c r="G61" s="78" t="n"/>
     </row>
     <row r="62" ht="15.75" customHeight="1" s="53">
       <c r="B62" s="16" t="n"/>
-      <c r="G62" s="79" t="n"/>
+      <c r="G62" s="78" t="n"/>
     </row>
     <row r="63" ht="15.75" customHeight="1" s="53">
       <c r="B63" s="16" t="n"/>
-      <c r="G63" s="79" t="n"/>
+      <c r="G63" s="78" t="n"/>
     </row>
     <row r="64" ht="15.75" customHeight="1" s="53">
       <c r="B64" s="16" t="n"/>
-      <c r="G64" s="79" t="n"/>
+      <c r="G64" s="78" t="n"/>
     </row>
     <row r="65" ht="15.75" customHeight="1" s="53">
       <c r="B65" s="16" t="n"/>
-      <c r="G65" s="79" t="n"/>
+      <c r="G65" s="78" t="n"/>
     </row>
     <row r="66" ht="15.75" customHeight="1" s="53">
       <c r="B66" s="16" t="n"/>
-      <c r="G66" s="79" t="n"/>
+      <c r="G66" s="78" t="n"/>
     </row>
     <row r="67" ht="15.75" customHeight="1" s="53">
       <c r="B67" s="16" t="n"/>
-      <c r="G67" s="79" t="n"/>
+      <c r="G67" s="78" t="n"/>
     </row>
     <row r="68" ht="15.75" customHeight="1" s="53">
       <c r="B68" s="16" t="n"/>
-      <c r="G68" s="79" t="n"/>
+      <c r="G68" s="78" t="n"/>
     </row>
     <row r="69" ht="15.75" customHeight="1" s="53">
       <c r="B69" s="16" t="n"/>
-      <c r="G69" s="79" t="n"/>
+      <c r="G69" s="78" t="n"/>
     </row>
     <row r="70" ht="15.75" customHeight="1" s="53">
       <c r="B70" s="16" t="n"/>
-      <c r="G70" s="79" t="n"/>
+      <c r="G70" s="78" t="n"/>
     </row>
     <row r="71" ht="15.75" customHeight="1" s="53">
       <c r="B71" s="16" t="n"/>
-      <c r="G71" s="79" t="n"/>
+      <c r="G71" s="78" t="n"/>
     </row>
     <row r="72" ht="15.75" customHeight="1" s="53">
       <c r="B72" s="16" t="n"/>
-      <c r="G72" s="79" t="n"/>
+      <c r="G72" s="78" t="n"/>
     </row>
     <row r="73" ht="15.75" customHeight="1" s="53">
       <c r="B73" s="16" t="n"/>
-      <c r="G73" s="79" t="n"/>
+      <c r="G73" s="78" t="n"/>
     </row>
     <row r="74" ht="15.75" customHeight="1" s="53">
       <c r="B74" s="16" t="n"/>
-      <c r="G74" s="79" t="n"/>
+      <c r="G74" s="78" t="n"/>
     </row>
     <row r="75" ht="15.75" customHeight="1" s="53">
       <c r="B75" s="16" t="n"/>
-      <c r="G75" s="79" t="n"/>
+      <c r="G75" s="78" t="n"/>
     </row>
     <row r="76" ht="15.75" customHeight="1" s="53">
       <c r="B76" s="16" t="n"/>
-      <c r="G76" s="79" t="n"/>
+      <c r="G76" s="78" t="n"/>
     </row>
     <row r="77" ht="15.75" customHeight="1" s="53">
       <c r="B77" s="16" t="n"/>
-      <c r="G77" s="79" t="n"/>
+      <c r="G77" s="78" t="n"/>
     </row>
     <row r="78" ht="15.75" customHeight="1" s="53">
       <c r="B78" s="16" t="n"/>
-      <c r="G78" s="79" t="n"/>
+      <c r="G78" s="78" t="n"/>
     </row>
     <row r="79" ht="15.75" customHeight="1" s="53">
       <c r="B79" s="8" t="n"/>

</xml_diff>